<commit_message>
Get daily reddit data: Mon Sep  9 08:11:35 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_09_15.xlsx
+++ b/data/collected_data/2024_09_15.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C320"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,329 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1fcjoxd</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>Rubber base gel without UV light?</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fcjoxd</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1fcjbih</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>Dip ombre</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d2l3xagceqnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1fcjam7</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Spooky nails </t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fcjam7</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1fcj4i4</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail Removal Etiquette </t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fcj4i4/nail_removal_etiquette/</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1fciz8r</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t xml:space="preserve">vacay nails! Dried flowers🌸💮 Cute for brides too. 🍂 </t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tgvchebr9qnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1fciuy0</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>Simple toenails, what do you think?</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l2a6w0188qnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1fci2gk</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How do I make my nails look better? </t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fci2gk</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1fcipbk</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The Iron Fist Of The Working Class Breaking Through The Crust </t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fcipbk</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1fchz48</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t xml:space="preserve">French + cherries 🍒 </t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j05mec6expnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1fchaaf</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t xml:space="preserve">sooo in love with this matching set 🩷 </t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fchaaf</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1fch4pm</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>What's a substitute for OPI rapid dry? It's discontinued</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fch4pm/whats_a_substitute_for_opi_rapid_dry_its/</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1fcgwtq</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>🐢💓</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t8jyvi8olpnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1fcij6n</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>Has anyone used this or other steam gel removers? I want to try it but it seems too good to be true</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cl2ox7vy3qnd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1fci8j9</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>Shrinkage</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8scmudsg0qnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1fch7dt</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>dude. i am so done with mooncat</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fch7dt</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1fcgwcx</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>Nails wrecked from gel-is shellac safe?</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fcgwcx/nails_wrecked_from_gelis_shellac_safe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1fcj2py</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>I kept seeing a bunch of Beetlejuice inspired sets, so here’s my take! The green drips glow in the dark 💕</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qu569kk1bqnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1fcigsq</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>Fruit Picnic 🍓🍒🍋🍊🥝🫐🍇</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/76thrzga3qnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1fchytf</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t xml:space="preserve">French + cherries 🍒 </t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i7msgguaxpnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Tue Sep 10 08:10:10 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_09_15.xlsx
+++ b/data/collected_data/2024_09_15.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C320"/>
+  <dimension ref="A1:C492"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5873,6 +5873,2930 @@
         </is>
       </c>
     </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1fdcng8</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I just got some new press-on nails that are handmade and super pretty, but they're a bit too small. Any tips on how to figure out the right size for me? </t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fdcng8</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1fdbrhm</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>Very demure, very mindful ✨️ Is this nail shape ok though?</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fdbrhm</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1fdb6td</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>New design, I hope you like it and let me know what you think</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zxfomyfecxnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1fdb3k0</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t xml:space="preserve">More spoopy mails! spider was here? </t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fdb3k0</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1fdazfw</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Trying some bold new styles (at least for me) </t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/donxxrbt9xnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1fdavd6</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>Winter Pedicure ideas</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fdavd6/winter_pedicure_ideas/</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1fdastm</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>GelX Cat Eye set… just got them done today and I am in love!!</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fdastm</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1fda0s4</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>Can't believe my natural nails looked like this before):</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dxy30f46ywnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1fd9gs3</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>Any dupes for OPI Cherry Blossom?</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2u7q5v41swnd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1fd8lpa</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Colorful nails, what do you think? </t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x2bilm63jwnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1fd8hrk</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>Do these look as bad as i feel they do?</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fd8hrk</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1fd8gom</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>Got my nails done</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fd8gom</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1fd8fl3</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t xml:space="preserve">end of summer nails </t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ilscwcafhwnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1fd7igb</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>Do I have "good" nail beds?</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fd7igb</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1fd7wy2</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Rogue Lacquer - Haunted Holiday </t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fd7wy2</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1fd7sxl</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail Polish Simply doesn’t dry </t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fd7sxl/nail_polish_simply_doesnt_dry/</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1fd7mij</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>Elegance❤️what do girls think?</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xhq1m3tt9wnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1fd7kj5</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>As someone who has a job where I can’t have acrylic nails I’m so happy press ons have become more quality and popular and I can have nails on the weekend now!</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fd7kj5</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1fd7gh2</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>RUSSIAN GEL MANI IN WHITE 🤍</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u47f24ba8wnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1fd6zmm</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New to nails, first fill </t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r9uyqs8y3wnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1fd6yng</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>Beetlejuice Beetlejuice Nails</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fd6yng</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1fd6vrx</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>My perfect autumn nails 🤎</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/obpva0ty2wnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1fd6r4z</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>Cute??? 💅</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/89j97gft1wnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1fd6pxd</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>File before fill?</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f2kjwdgi1wnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1fd5xn2</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>NYC Experienced Nail Tech Rec Needed</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fd5xn2/nyc_experienced_nail_tech_rec_needed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1fd61zb</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Press On vs Builder Gel for short nails </t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fd61zb/press_on_vs_builder_gel_for_short_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1fd5u3k</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>Monday Mani compliments of my new nail tech. Please, no hate. She's not even 2 yet 😅</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fd5u3k</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1fd5q49</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>Tis Almost Fall!</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fd5q49</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1fd5gjh</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>Is there any way to fix this?</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3tzo535aqvnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1fd56r6</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Semi-Twinning w My Bestfriend for Our Graduation🥰 </t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fd56r6</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1fd538u</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>What is a shellac change?</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fd538u/what_is_a_shellac_change/</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1fd50ox</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>Trying to liven up my shorties, what do you think?</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fd50ox</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1fd1an8</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>Loving the red this fall</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fd1an8</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1fd4u4b</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>🍁♥️🍂✨</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qq13tj2skvnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1fd4tbt</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>My nail tech fulfilled my whimsical dreams 🍄✨</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m2quby9lkvnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1fd4gw8</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>Slowly getting better at doing my own nails</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ifm9ny4mhvnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1fd3nvs</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>Friends wedding nail colors</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9lg9rmrpavnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1fd3iqv</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My first time trying gel! :) 🫧 </t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e2d8k13l9vnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1fd3fo7</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>In need of serious help</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fd3fo7</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1fd330g</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>my best friend is learning how to do nails! this time we did a brat (charli xcx theme) and she did so good!!!</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ewesr1u26vnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1fd23ii</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t xml:space="preserve">because here from anywhere 🌹 </t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xwlo5a81yund1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1fd1x6a</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>Have you heard about the red nail theory? What do you think about that🤔🤗</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fd1x6a/have_you_heard_about_the_red_nail_theory_what_do/</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1fd0uot</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t xml:space="preserve">my last works were a bit crazy 🤣 so i decided to do a simple french. but it's still not simple... what do you think? </t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fd0uot</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1fd0t47</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>fiery halloween tips</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fd0t47</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1fd0kt3</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>Seeking manicure advice</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fd0kt3/seeking_manicure_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1fd0j8t</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>my second set ive ever done!!</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tn9k5vqdmund1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1fd0i7a</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>WHY CANT I STAMP!!</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ptyolil6mund1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1fd0gp7</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>Monarch Butterfly Nails</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fd0gp7</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1fd0b8x</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Poly Gel Set </t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5jhraexukund1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1fd028a</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>Can’t get enough of my exaggerated frenchies</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/om56m5t0jund1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1fcz444</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>My holiday set 💖</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fcz444</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1fcznsh</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Best set yet… </t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fcznsh</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1fczhht</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>Natural nail growth journey :)</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fczhht</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1fcz1pj</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>New press ons 😍</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bzuied2qbund1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1fcyw2j</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Trying out Dashing Diva GelXtend nails from Sally’s. </t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/je8m863naund1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1fcyu7j</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I spilt liquid acrylic on my couch’s cup holder things and it melted the plastic </t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jxlte5yaaund1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1fcynfx</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>some cute hello kitty nails 🎀 (don’t ask me about my other hand lmao)</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fcynfx</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1fcxs8m</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Broken nails </t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fcxs8m</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1fcydch</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>DOES ANYONE KNOW WHAT SHADE OF NAIL VARNISH THIS IS inspo pic for pinterest @tatiana</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zjbf3fsw6und1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1fcyds4</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Brown szn </t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fcyds4</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1fcy8zu</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>stickers from amazon</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o6ibyz526und1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1fcy5rp</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>Ways to pay friend for doing nails</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fcy5rp/ways_to_pay_friend_for_doing_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1fcy48t</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>How should I shape my nails?</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fcy48t</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1fcxyx3</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Do I need a break from acrylics? </t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nz854zd44und1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1fcxrk1</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>the golden sparkles gave it the touch</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/js0snsmp2und1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1fcxl3y</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>Which nail polish would closest to this color? Not my pictures/hands</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fcxl3y</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1fcx8pl</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Stuck with square? </t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fcx8pl</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1fcwovu</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>Which colour is better?</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fcwovu/which_colour_is_better/</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1fcwv7v</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>What gel colors to use to achieve this look from Mooncat?</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zqho99p8wtnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1fcwpra</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>Rund 2: Almond Or Coffin/Ballerina?</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i9klyew5vtnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1fcvp9h</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>What nail shape and length would look best on my hand?</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xfhe7ymsntnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1fcvc2n</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t xml:space="preserve">From a scale of 1 to 10 how obvious is it they are press Ons? </t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fcvc2n</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1fcui6w</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My bear is really cute </t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8br1d49vetnd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1fcueal</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>Impress Wanderlust</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fcueal</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1fcu0fb</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>My first time trying ombre..</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/52v71uaabtnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1fctclq</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>Do you like them? I think next time I'll do something not so classic</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/779u9g3f6tnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1fcsy6c</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>The perfect pumpkin orange with gold shimmer!</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ejiwvndk3tnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1fcsw5b</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail progression </t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fcsw5b</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1fcsv0n</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>September nails 🧿✨</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fcsv0n</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1fcro3j</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>Fantasy nails to transition to fall</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fcro3j</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1fcl2pz</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>Curved lines on nails after manicure?</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/my9zrjmi2rnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1fcm87n</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>Anyone tried tips from shein/temu</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fcm87n/anyone_tried_tips_from_sheintemu/</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1fcmdst</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>My 16 year old did my nails</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/32l2z8d9jrnd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1fcr72u</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>French fills?</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fcr72u/french_fills/</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1fcr2bh</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>Happy Spooky Season, all! Enjoy my Pennywise set!</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/60el9prjpsnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1fcqvn6</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>Peeeeearl 😍😍😍</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fcqvn6</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1fcqu34</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>practicing press on nails !</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fcqu34</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1fcqso0</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t xml:space="preserve">One of these things is not like the other </t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zxbfwckgnsnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1fcqn93</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>Still 80° here but was too excited to try some fall chrome</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fcqn93</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1fcqbz1</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Missed the glue on’s </t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7jp6xauvjsnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1fcoyfk</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>I'm looking for Halloween designs, can you help me?</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/11g9bq6g8snd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1fcojue</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>My new 💙</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n90vbesy4snd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1fcnjsa</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My nails after cutting into shape and after shaping </t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fcnjsa</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1fcn3fu</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t xml:space="preserve">best way to stick press on nails? </t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fcn3fu/best_way_to_stick_press_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1fcmwee</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>September chrome!💅✨</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/43xihjj1prnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1fcmifa</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Polish recommendations/application tips to get this kind of look? </t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fcmifa</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1fcm9so</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>Birthday Set</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fcm9so</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1fckxnf</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t xml:space="preserve">By me, on me. Dont know how i feel about them! </t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fsp6o4wo0rnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1fdckx7</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>Short n sweet 🍒</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fdckx7</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1fdafw9</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>this is what happens when you move in to a new place😭</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fdafw9</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1fd9d6q</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>🍂Cirque Eye of the Beholder🍁 (velvet)</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/dhkgpqjxqwnd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1fd8f2i</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>I can't justify PPU for one polish, please help me dupe</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nqg9wbbahwnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1fd80of</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Rogue Lacquer - Haunted Holiday </t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fd80of</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1fd7kxd</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>Pics don’t do this justice ✨🌌</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fd7kxd</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1fd77bz</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Super shifty, color identity crisis </t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fd77bz</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1fd6r1a</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>Clionadh anniversary sale haul</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fd6r1a</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1fd6ecy</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>Looking for a dupe!</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ajj7alumyvnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1fd4ytv</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>Layering experiment fun!</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fd4ytv</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1fd4vq0</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>Glitter and thermal polishes on my xs shorties 🩷💜💖💅</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fd4vdh</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1fd4oam</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>🍁♥️🍂✨</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cavwse5ejvnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1fd4be8</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>Green Skittle</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fd4be8</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1fd3x8a</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Does anyone here have tips regarding moving with your large collection? </t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fd3x8a/does_anyone_here_have_tips_regarding_moving_with/</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1fd3sku</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>This color makes me feel much more put together than I actually am</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fd3sku</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1fd3amp</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail art inspired by my favorite mug </t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fd3amp</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1fd384v</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>Anyone try this polish before?</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mlnj09x47vnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1fd2ksn</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>SPOOKY TIME</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fd2ksn</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1fd2c7c</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>Matcha Cloud ☁️</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fd2c7c</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1fd121x</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>Any recommendations for speckled polishes like ILNP's?</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fd121x/any_recommendations_for_speckled_polishes_like/</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1fczjn1</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Vampy french tips </t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fczjn1</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1fcz5mp</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Allergies - gel &amp; nickel alternatives </t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fcz5mp/allergies_gel_nickel_alternatives/</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1fcybrq</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>Best opaque gold metallic polish for freehand linework?</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fcybrq/best_opaque_gold_metallic_polish_for_freehand/</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1fcy3ds</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Favorite brands that do Afterpay and Klarna? </t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fcy3ds/favorite_brands_that_do_afterpay_and_klarna/</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1fcx9dc</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mooncat sales/ PPG? </t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fcx9dc/mooncat_sales_ppg/</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1fcvtrk</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>Took my nails out on a hazy hike and it really brought out the shimmer!</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fcvtrk</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1fcvlcq</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>Quality glow in the dark gel?</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fcvlcq/quality_glow_in_the_dark_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1fcvcnh</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>I love a good glow🌟</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fcvcnh</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1fcv5cs</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>I used the horseshoe magnet but it still came out splotchy. What am I doing wrong?</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/uaelpmrojtnd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1fcuxxs</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>Voyage Hues, going the distance!</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2t2cum26itnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1fcut3p</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Swamp Sparrow, Two Ways </t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f5vngvy4htnd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1fcuqq5</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>Ghoblins and Ghoulies 😍</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fcuqq5</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1fcuq64</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>shiftyyy</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fcuq64</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1fcudgl</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>Ending the summer mani season on a high note</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fcudgl</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1fcub8w</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>Lil ilnp haul</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fcub8w</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1fcu24d</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>in space no one can hear you scream</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fcu24d</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1fctveb</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>Calathea nails</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/73pfvi88atnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1fctn3k</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>Curved lines on nails after manicure?</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/faaoku4j8tnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1fct9iq</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>Jade Jelly</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4jknusnt5tnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1fct5sx</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>Cheap polish suggestions.</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fct5sx/cheap_polish_suggestions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1fcsx0h</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>The perfect pumpkin orange with gold shimmer!</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/520ukekb3tnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1fcsp0q</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>Glowy Iridescent 🫧</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fcsp0q</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1fcs74o</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>*SPOILERS* Lurid Lacquer's Halloween Advent</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fcs74o</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1fcqx2r</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>This is a travesty. How do I fix it?</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ncaz5ncfosnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1fcqplp</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>A sheer lit from within look</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fcqplp</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1fcqos9</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>10 year old son was bullied for his nails</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jrhj5ebnmsnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1fcq9h6</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>Holo Taco Pink Smoothing Base + Everything Taco | Beautiful Result, Frustrating Application</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fcq9h6</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1fcq64e</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>How often is it adviced to go between appointments?</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fcq64e/how_often_is_it_adviced_to_go_between_appointments/</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1fcpb74</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>Please help me with my damaged nails. What can I do?</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/re6rgjpkbsnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1fcp5kd</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>Anyone have some dupes for these 4? I don't want to buy from Mooncat...</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fcp5kd</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1fcnh4t</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>Blazing Evening Sky</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fcnh4t</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1fcng8m</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How do you properly prep cuticals and the nail bed? </t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fcng8m/how_do_you_properly_prep_cuticals_and_the_nail_bed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1fcn1th</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>Frosted Light</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fcn1th</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1fcmfs4</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>Cool Toned BRIGHT Red?</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fcmfs4/cool_toned_bright_red/</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1fcm0ln</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>Looking for Essie From a to zzz colour</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lrhrb9rrernd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1fcluf6</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>Brown color</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fcluf6</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1fclrwd</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fclrwd/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1fclctu</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>Hey, UK lacqueristas! Where do you buy your Zoyas from?</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z3u3035d6rnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1fdbk89</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A couple of my sets throughout the years </t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fdbk89</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1fdb3m4</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t xml:space="preserve">More spoopy mails! spider was here? </t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fdb3m4</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1fd9yij</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>Where to get nail supplies brushes etc</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1fd9yij/where_to_get_nail_supplies_brushes_etc/</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1fd6h99</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>sky blue or pearl white for diy french tip?</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4cktm429zvnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1fd19sa</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Strawberry Nails 🍓 </t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fd19sa</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1fd0eds</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>Monarch Butterfly Nails</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fd0eds</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1fcxei6</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>Rate my GFs first set of Acrylic nails</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/26ba77x50und1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1fcuoei</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My favourite nail sets in a while </t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fcuoei</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1fcueoq</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>3D-printed magnetic nail art stand</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fcueoq</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1fcuejc</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>~👀 Lowkey, went with the F̶l̶o̶w̶ Dots 。。。</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zrqnn5v5etnd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1fcrriy</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>Nail Pigment Powders/Eyeshadows???</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1fcrriy/nail_pigment_powderseyeshadows/</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1fcrizn</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>Pennywise! Happy Spooky Season!</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/19urlqe3tsnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1fcqqgs</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>When it’s really time to let them go but they took you so long to make and you don’t have the guts now</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fcqqgs</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1fcqof6</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>Frog nails 🐸</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fcqof6</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1fcqb1r</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>hello kitty cheetah nails!! 🩷✨</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fk63d3sojsnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1fckppw</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>Recent diy meme manicure and with colorful</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tgwkuhmfxqnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Sep 11 08:10:16 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_09_15.xlsx
+++ b/data/collected_data/2024_09_15.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C492"/>
+  <dimension ref="A1:C648"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8797,6 +8797,2658 @@
         </is>
       </c>
     </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1fe445v</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>I did some spiders and rainbow ombre web nails.</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fe445v</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1fe427t</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>Acrylics for lifelong nail biter</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fe427t/acrylics_for_lifelong_nail_biter/</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1fe3r26</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>paid $65. i like it but what do y’all think?</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tbqsmpall4od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1fe2krw</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help me find this nail polish shade? inspo from @gelfullynails on YouTube </t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f6xbcmz674od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1fe3cfa</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>Best nail/cuticle oil</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fe3cfa</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1fe37la</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>Early Fall nails 🍂🐆</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0ygn6uhte4od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1fe31oa</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>Maybe these on Friday 😍</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pis8gk9vc4od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1fe2gim</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>Japan Ready!</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ggflbqbs54od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1fe1xm0</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Grunge/rockstar nails for my guitarist friend :) </t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3pt8vly104od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1fe1wo0</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>Some leopard I did for my friend!</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s39nno7sz3od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1fe1sj0</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My hen do nails </t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pkvds46hy3od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1fe10dd</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>Check my new set 🖤</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fe10dd</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1fe0wpb</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fe0wpb/chrome/</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1fe0afo</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>This color looks like a nude color? I love the design</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/pzxj6z4fj3od1</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1fe01nk</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>😎 Dirty 30’s 🎂</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8uetsfd3h3od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1fe00n6</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t xml:space="preserve">🌀 UMF 24’ 👽 </t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6r2e97mtg3od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1fdyxyh</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t xml:space="preserve">When you hit it on just the right angle </t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fdyxyh</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1fdvlcx</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t xml:space="preserve">nail sticker recs? by me &amp; crew nails thoughts </t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fdvlcx/nail_sticker_recs_by_me_crew_nails_thoughts/</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1fdpzgd</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>Press on nail size order issue</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fdpzgd/press_on_nail_size_order_issue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1fdp8zu</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>New set!</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fdp8zu</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1fdznbq</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>"Y" or " N"</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vjm0gjd8d3od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1fdzln0</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Solid bright pink, or add holo chunkies? </t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fdzln0</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1fdz8f8</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time getting chrome </t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k36z80fd93od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1fdytzi</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>All Hail The Pumpkin King</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4qhi01fk53od1</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1fdym6q</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nails Too Sharp? </t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5hyasdca33od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1fdy4t6</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>Love my little soot sprites 🥰</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2qqiqe7py2od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1fdxpn8</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>2nd layer of gel peeling off 1st…why?</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xszrb8ctu2od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1fdx48d</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>Black frenchies🖤🖤</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fdx48d</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1fdx3l9</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>Cute pink set🩷🩷</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fdx3l9</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1fdwy5r</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Happy Tuesday 🎶✨️Love my new nails💓 </t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oges5yf1o2od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1fdwn9f</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>I just did this nail cleaning.</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vxpicxjal2od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1fdw89k</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Colour choice? </t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tqjqousth2od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1fdvu9y</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mani, gel mani, or gel x? </t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fdvu9y</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1fdvflp</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Got my nails done today! </t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fdvflp</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1fdvckw</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>Help with Gel Lamp</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i0gomknga2od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1fduwu7</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t xml:space="preserve">too pretty not to share the beautiful nails of my friend, Amari </t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7116p5kk62od1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1fduki5</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>Thoughts? 🎀</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1m75ansz32od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1fdtyb1</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>How do you get topper glitter coats to work?</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fdtyb1/how_do_you_get_topper_glitter_coats_to_work/</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1fdtxqy</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>Nothing better than some happy nails to lift my spirits</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9y0ydh41z1od1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1fdpd96</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>Gel nails - is it possible to form all the nails first and then curate?</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fdpd96/gel_nails_is_it_possible_to_form_all_the_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1fdswnx</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>best products for gel x</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fdswnx/best_products_for_gel_x/</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1fdsuzn</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>SOBBING 😭</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7k867yorq1od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1fdsi1z</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>How’d I do?</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/70552b33o1od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1fds3s8</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>just realized we match! 🐱💅</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hlnlaoc3l1od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1fdqdkk</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>Gelish - Inhibition Layer</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fdqdkk/gelish_inhibition_layer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1fdqih0</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Game inspired nails - Hollow knight </t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fdqih0</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1fdqnh6</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>Long Awaited Nails</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fdqnh6</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1fds0gh</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>Obsessed with how these turned out!</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wlezdj4gk1od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1fdq0mn</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>Is gelx really "better" for your nails and is there evidence of that? Just curious!</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fdq0mn/is_gelx_really_better_for_your_nails_and_is_there/</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1fdq0e8</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t xml:space="preserve">pure perfection of new manicure </t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1bl2h1js51od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1fdptpe</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Never posted my august amethyst geode nails 💅 </t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fdptpe</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1fdpqmk</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pallet cleanser after summer to transition to fall ✨ </t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fdpqmk</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1fdpowo</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>nail designs for stubs?</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fdpowo/nail_designs_for_stubs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1fdpeg9</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>🐆❤️‍🔥</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c2mek9ed11od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1fdpchn</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>Beetlejuice Inspired Nails 2.0</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c4z3pn3y01od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1fdpbr5</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>Beetlejuice Inspired Nails</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oaa07mnr01od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1fdp46z</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>Megan Thee Stallion NEVA PLAY Inspired Nails</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/h5mrvay7z0od1</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1fdoo99</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>New temu press ons</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bhbye454w0od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1fdo83r</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Just simple 💅🏻 </t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7a8n7q3ws0od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1fdna9w</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>What kind of nails should I get?</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fdna9w/what_kind_of_nails_should_i_get/</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1fdnwa5</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>added some charms! what do you think?</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s5pkvr2eq0od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1fdnovb</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>New set 😫</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rsjc1un1p0od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1fdndej</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>Is beetles really that bad?</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qr6mda3sm0od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1fdn45i</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>I got DRAGGED last time I posted my nails about my cuticles. Y’all happy now?😂🫶</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/el5nhlqxk0od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1fdn245</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>First time doing ombré and hand-painting a design! Cat eye over gel polish, builder gel extensions</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5osn4s0jk0od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1fdn10e</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>a little help</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fdn10e/a_little_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1fdmveu</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>Two sets I finished yesterday! 🖤</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fdmveu</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1fdmtyh</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nude Pink Acrylic with Aqua Pink Gel Top Coat on both 💗 </t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fdmtyh</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1fdmebf</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>Spooky vibes 🏚️👀☠️</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fdmebf</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1fdm2tu</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>Tried chrome nails for the first time</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ib994rtcd0od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1fdlicu</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>In Brazil!</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i605l12590od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1fdl009</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>I did these nails, did they turn out okay?</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jdyywb6g50od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1fdkyxx</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is it possible to cap the tip/edge with paint without getting paint underneath the nail? </t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fdkyxx/is_it_possible_to_cap_the_tipedge_with_paint/</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1fdd4k0</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>OPI long wear polish or Essie gel couture?</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fdd4k0/opi_long_wear_polish_or_essie_gel_couture/</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1fdfxes</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>Post acrylic damage , how long before new set ?</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fdfxes</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1fdk7jn</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>Polka Dot Fun</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hrp6xb3pzznd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1fdjx7r</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>👻🌸Spooky Nails🌸👻</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nbwoc1fkxznd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1fdj3xm</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>Kiss IMpress nails—can you paint?</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3otnlgucrznd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1fdj1zf</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Wedding Manicure, what do we think?  </t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2u40ccrxqznd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1fdiuew</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>How could I Improve my nails? I ALWAYS have trouble around my cuticles &amp; have to file around them</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6o19ckc9pznd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1fdieo3</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>Finally got my nails done after 3 months! ❤️</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0e47hkoplznd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1fdi5po</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> First Time Getting My Nails Done - How did they Do?</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fdi5po</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1fdhznz</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>All Hail The Great Lord Rimuru 😋</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fdhznz</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1fdhjwt</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>🧜🏽‍♀️ vid</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/w3oi8xvseznd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1fdgtbi</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>Birthday Nails 🎂</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fdgtbi</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1fdgnzr</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>🧜🏽‍♀️went to a mermaid party, so I figured why not! Lol</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fdgnzr</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1fdghhu</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gel mani on mom! </t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ol427aig5znd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1fde5eh</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t xml:space="preserve">love this color scheme… picked oh so carefully 🤭 shaped and painted myself. 💋 welcome to my signature look! </t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/gs0jtsv5gynd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1fddfk8</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>Cat eye - yay or nay?</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fddfk8</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1fdddu4</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>Light freckles under nail?</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fdddu4</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1fe1413</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>Can we figure out the VP's mani?</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fe1413/can_we_figure_out_the_vps_mani/</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1fdykjp</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>Dupe for Chanel Phénomène?</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/84qcaqn033od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1fdykbr</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First polish I want to buy a backup for. “Don’t Guava Clue” from Painted Polish. It’s my favorite color I’ve worn yet and I want more plus all the colors from the collection. Just drown me in glitter crellies. </t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fdykbr</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1fdyd7e</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>Lil Lizard</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fdyd7e</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1fdy3jo</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Did Essie change the formula of Turquoise and Caicos? </t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fdy3jo</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1fdy2zd</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>Sunset Nails 🌅</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/r1f9k1c6y2od1</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1fdxdf9</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>Miss Argentina nails🧟‍♀️</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7a016xurr2od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1fdwrqg</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>idk who needs to hear this, but…</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ethdyehm2od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1fdvo5x</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t xml:space="preserve">first fall mani of the season </t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7jtm86c4d2od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1fdvb9b</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>Transition into autumn colours🍃</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gikw0v95a2od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1fdv1eh</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>Tragedy strikes...</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fdv1eh</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1fduzwg</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>Indies Down Under Chat</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fduzwg/indies_down_under_chat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1fduqrg</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Got something new coming in the mail today so I’m taking these off right after work lol. It’s overcast out sorry for the not so great pic. </t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qzbff18e52od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1fdup93</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>Kbshimmer - Apple-y ever after</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fdup93</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1fdt8v1</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dupe Request Holo Taco Devil's Advocate </t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fdt8v1/dupe_request_holo_taco_devils_advocate/</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1fdsy0i</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>First Mooncat order 7 colpir skittle to test. 1 holotaco nail for balance</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ehka4a2er1od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1fdscnl</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>Cirque colors Linen dupe?</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s2a15crxm1od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1fdqxp9</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t xml:space="preserve">mooncat’s response to my exploded bottle </t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fdqxp9</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1fdqb6r</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>Which color looks better?</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fdqb6r</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1fdo9md</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Anyone know a dupe of Mooncat Dark Horse? </t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s8ux2h37t0od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1fdo36j</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>Non-gel blooming polishes?</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fdo36j/nongel_blooming_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1fdnzbj</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>First Emily de Molly</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fdnzbj/first_emily_de_molly/</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1fdnm88</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>Why is car lighting so good for nailfies 💜</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fdnm88</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1fdnekw</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>Clionadh GWPs?</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fdnekw</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1fdnall</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New nail shape </t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kxr8uu28m0od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1fdn5x1</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>Matte fun</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fdn5x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1fdn3ry</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>"We have nail polish at home"</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/we-have-nail-polish-home-fXI6FVF</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1fdmx63</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>First Bottle of Bee's Knees 🐝</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xc8tuk9jj0od1</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1fdlq2c</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>Zoya z wide brush too long for ILNP bottle?</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fdlq2c/zoya_z_wide_brush_too_long_for_ilnp_bottle/</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1fdlm0b</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>What is this? It doesn't go away when I shake the bottle. It's never used, and looked normal when it arrived. Now it's been white for a few months already.</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fdlm0b</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1fdlgy0</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>Starry sky vibes!</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fdlgy0</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1fdl2ft</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>Where do you like to shop second hand polish?</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fdl2ft/where_do_you_like_to_shop_second_hand_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1fdkfsf</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t xml:space="preserve">my little collection </t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fdkfsf</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1fdjs8g</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>ILNP Sirene 🧜‍♀️</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/m5hdugyhwznd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1fdjjys</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>Autumnal Plaid</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fdjjys</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1fdjixz</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>How to get tie dye off nails?? Already tried washing and shower didn’t help</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jr4c8rdduznd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1fdixpv</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Glowing blue/coppery/golden skittle </t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fdixpv</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1fdiwe3</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>One of the most beautiful polishes I've worn</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fdiwe3</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1fdisww</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>Fancy Gloss Mystery Box?</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fdisww/fancy_gloss_mystery_box/</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1fdiq3x</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>New Bottle Update y’all</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fdi2vj</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1fdhfvp</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>You’ve heard of Christmas in July, please allow me to present: St. Pats in September!</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/sf3WIEN</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1fde6wg</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>HHC Monthly Megathread</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fde6wg/hhc_monthly_megathread/</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1fddhwb</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>I didn't plan these nails, but I love them!</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fddhwb</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1fe42fp</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>Beetlejuice 🪲 🧃</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fe42fp</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1fe3kc2</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Any tips to make it look better? </t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1fe3kc2/any_tips_to_make_it_look_better/</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1fe0vkd</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>Last summer set, feel kinda ehh about them lol 🤷🏻‍♀️</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/slcp1ce2p3od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1fe01wg</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>Are These Elegant Textured Enough for My Nails?</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pmp7lo4qg3od1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1fdzsmf</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I feel like I've aged 10 years painting these! </t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fdzsmf</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1fdydyv</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Bold Glitter and Colorful Nails </t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rmu5tpo413od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1fdxcq6</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>My second try at doing cartoon nails</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5zfl9o6kr2od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1fdvqqn</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Halloween inspired nails on my best friend </t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eahvzoipd2od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1fdvcx5</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>Bumblebee nail set</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3p4g2ohja2od1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1fdv6r8</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>Did this set on my sister in law. Is it too pink that you cant see the details?</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wgtgs2hy82od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1fdtvpm</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>Angel/Renaissance ❤️😇</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4g4fkvhly1od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1fdsk4i</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>so proud of these 🥹</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yypt9fsio1od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1fdrarm</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>Sculpted in gel and nail art🩷</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nmizq4e7f1od1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1fdqsth</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t xml:space="preserve">new to nails </t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1fdqsth/new_to_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1fdpao5</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t xml:space="preserve">i can’t stop posting about these 😩 </t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fdpao5</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1fdmhx5</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>Last gel summer set!</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fdmhx5</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1fdl01j</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>Spider gel fun</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fdl01j</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1fdkwuv</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time using g nail foils </t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fdkwuv</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1fdksij</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t xml:space="preserve">DIY handmade gel nails </t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fdksij</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1fdknpk</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Handmade gel nails </t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fdknpk</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1fdkbr9</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>Hand painted Halloween nails</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fdkbr9</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1fdk9e1</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>Halloween nails</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fdk9e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1fdi0t3</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>🧜🏽‍♀️went to a mermaid party, so I figured why not! Lol</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fdi0t3</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Sep 12 08:10:14 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_09_15.xlsx
+++ b/data/collected_data/2024_09_15.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C648"/>
+  <dimension ref="A1:C822"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11449,6 +11449,2964 @@
         </is>
       </c>
     </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1fewxlk</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>Vacation nails 🌊</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fewxlk</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1fevxdg</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>Beetlejuice x Bob's Burgers 💚</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fevxdg</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1fevnd1</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>Chameleon chrome nails</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fevnd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1fev6bz</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ready to get through another work week ✨ </t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g2m0c73qebod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1fev4um</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>Nail tech did such a good job!!</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fev4um</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1fetyak</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t xml:space="preserve">garden of eden freestyle </t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fetyak</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1fetqj0</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>Beginner nail artist, teaching myself gel x and finally feel like Im improving</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ae7lcmzsyaod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1fetmxy</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>today ✨❤️</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/28auutvuxaod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1fet83b</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t xml:space="preserve">can i file and change the shape of press ons? and how? </t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h0nr7rkitaod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1fet3jo</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New nails </t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6und33y7saod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1feskz8</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Rubber base </t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1feskz8/rubber_base/</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1fes36q</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>Can anyone identify what polish this is? (credit - usanailmart) on youtube</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dt84qltciaod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1fes51u</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>First Halloween nails of the year!</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ym0m95bxiaod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1ferp21</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>After 2 weeks of filling the backs with nail glue and painting over them I finally got in with my new nail tech. Went simple for the first time but I love them!</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ferp21</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1fermax</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>An essential classic 💅</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jbw0ufs2eaod1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1ferktt</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>Espresso ☕️</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/tty69r1qdaod1</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1ferdce</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What’s a good gel polish brand that has breath taking cat eye colors? </t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ferdce/whats_a_good_gel_polish_brand_that_has_breath/</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1feqsmf</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>Thanks subreddit - fixed lol</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1feqsmf</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1fer3h4</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Charging friends </t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fer3h4/charging_friends/</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1feqvg3</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Custom Press ons done by my nail girl </t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1feqvg3</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1feqsg8</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>Got French tips with chrome over the top!</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/leowzvio6aod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1feq7cc</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t xml:space="preserve">to die for end of summer set </t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1feq7cc</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1fep8gz</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>here I leave this beautiful design</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x07hns7xs9od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1fep0jx</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My bridal nails! </t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fep0jx</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1feoelx</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>It finally happened😭</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s5dfnk3ul9od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1feoadk</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>New at nails, please let me know what I can improve on!</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1feoadk</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1fenrca</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>I found my people !</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pajskn7ig9od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1fenads</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>What is UP with my nails???</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fenads</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1femtmu</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>Dreading the right hand</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rr1j9fby89od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1femadq</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My most recent set </t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m1ohitlq49od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1fem14a</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>Jumping on the NUDE train!</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fem14a</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1felqdw</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>This color is so fall 🍂</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/e37i9nyd09od1</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1felnoj</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>Which way should nail art go??</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1felnoj/which_way_should_nail_art_go/</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1fektc8</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>New nails 💅🥰</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fektc8</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1feknvg</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>I’m so in love with this design &lt;3</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0cmyhggas8od1</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1fek40h</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>I got my nails done for the very first time ! What do you think ? + noob questions</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fek40h</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1fek3vp</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is this a bad manicure? </t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fek3vp</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1fej2pv</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>gel x done by me on myself</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fej2pv</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1feija5</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>I am now enrolled in nail school!</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1feija5/i_am_now_enrolled_in_nail_school/</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1fehpjp</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>Autumn gnone set</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fehpjp</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1fegxk9</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>It’s intended to be a holiday polish, but I think it’s beautiful for autumn!</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ufffcwcp08od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1fegrnf</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>Korean nail products really live up to the hype</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8v8uuachz7od1</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1fegdt8</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>new nailsss and a cat ive found</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fegdt8</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1fegc47</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>Last Summer Fruit Nails</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/073z481ew7od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1fefnvs</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>new to acrylic</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fefnvs/new_to_acrylic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1fefgtu</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>very delicate🎀</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/56iqw8v1q7od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1fefgh4</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>Nails in Albania</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fefgh4</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1fef5hu</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>Static Nails Mademoiselle - thoughts?</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fef5hu</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1fef450</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>Loving the cat eye gels recently!</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xej9wg3jn7od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1fef3d9</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>👽Glowy green💚</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fef3d9</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1feetto</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Some designs! </t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1feetto</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1feeqpk</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>Cheap chromes?</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1feeqpk/cheap_chromes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1feepma</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>KACHOW🏎️🏁</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1feepma</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1feegva</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>UV Lamp Question</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1feegva/uv_lamp_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1feeb4c</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>Throwback to some nails I made in 2021</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/dsinw8hoh7od1</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1fee5on</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>Matte or shiny?</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fee5on</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1fedzgs</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>Just tried Nail Thoughts builder gel and am currently obsessed. My</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fedzgs</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1fedl73</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>New rose gold nails</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fedl73</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1fedazb</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>New to Nails</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fedazb/new_to_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1fe49su</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>Onycholysis from acetone?</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lr4laudgs4od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1fe9f9n</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>1st and 2nd set of self-painted gel nails (my beautiful lumpys 🐫)</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fe9f9n</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1fe9knk</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Strongest base gel for gel x nails? </t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fe9knk/strongest_base_gel_for_gel_x_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1feac68</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>Should I wear press-ons instead of no chip for my wedding events?</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1feac68</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1feckly</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>Best Fake Nails for Small Hands?</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/78tjoh2157od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1fec3zf</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>Coralline nails</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fec3zf</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1feba9x</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>Gel top coat spots?</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1feba9x/gel_top_coat_spots/</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1feb8sd</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>Birthday nails 🍃💅🏻</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1feb8sd</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1featdk</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>tortoise shell french ✨🍂</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w5need8zr6od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1fe9z72</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>I wish all nail polishes and gels come in smaller/mini sizes</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o5fkbid6l6od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1fe9qov</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>another set I did myself!</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pvm7nox6j6od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1fe9eqs</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>new nails 🌊🫧</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fe9eqs</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1fe9eb4</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>Tried something new today</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7qhw9do8g6od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1fe9c3s</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>Beaux Rêves - Light My Fire 🕯️</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fe9c3s</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1fe871n</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>Essie Gel Couture</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fe871n</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1fe83xh</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>✝️ Rosary 🕊️</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kfcct9ta46od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1fe8371</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>EYE 🖤 U</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2fmh6bk346od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1fe7usz</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>I want to grow my hyponichium</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xdqfaksr16od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1fe7rsj</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>My sister is learning how to do nails by doing mine 🦋☁</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1lv3udlx06od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1fe755q</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t xml:space="preserve">my first time doing my own poly gel mani with cat eye gel </t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/04qa8g10u5od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1fe6l5q</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Just natural partner look with my daughter </t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s6t33zh2n5od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1fe5zme</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Most basic of the basics </t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e2zuvfdvf5od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1fe5z8j</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nails for my boyfriend </t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fe5z8j/nails_for_my_boyfriend/</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1fe5yuy</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>ILNP - Pink Lemonade</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fe5yuy</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1fe5qk3</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>I did them by myself</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zti4tze7c5od1.gif</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1fe51xl</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>more photos of my signature look :)</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fe51xl</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1fevq2l</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>Chameleon chrome nails</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fevq2l</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1fevl1k</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>Barbie Manicure</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fevl1k</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1fevgqk</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>Shoutout to Orly Customer Service</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ruxzn5l9ibod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1fev7sa</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>Anyone have MoonCat "Sand Viper" and Death Valley Nails "But Do Aliens Believe in me?"</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fev7sa/anyone_have_mooncat_sand_viper_and_death_valley/</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1feurxu</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>LIVING for the subtle nails right now</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1feurxu</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1fesyex</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>“Pre break” nails and swatches❤️❤️❤️❤️🌈 Sassy Sauce- Wet Spot</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fesyex</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1feswnf</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>Nail tech did me dirty</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1feswnf</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1fesgov</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>my nail growth progress 🖤</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d69vc2k1maod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1fes5b9</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>Rimmel Crushed Pearl</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fes5b9</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1ferok5</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>the perfect baby pink 🩷🎀</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ferok5</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1fermig</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t xml:space="preserve">long time lurker here 🥺 no-gel smoky quartz! </t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fermig</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1feqqi4</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>Loud lacquer - Alyssa</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ed2dsrb76aod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1feq4pp</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>Critiques invited</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ddu981us0aod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1fepkbq</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>PPU Rewind- Cameo Colours Lacquers Ghostly Guard</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5vgzgz9tv9od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1fepcxb</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>one of the most stunning polishes I have ever seen!!!!</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fepcxb</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1fep4hr</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>"Daylight curing" polish brands like Helios Luminor?</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fep4hr/daylight_curing_polish_brands_like_helios_luminor/</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1feol8q</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>I hate them 😫</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/puaornlfn9od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1feojxc</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cracked pink neutral skittle </t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9f87fvw3n9od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1feoi9a</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>Pulled Out my Magnets</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1feoi9a</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1feo8mt</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>First attempt at nail art!! Any tips?</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/prd3lcifk9od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1fenmpb</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>some of yall NEED to see this!!!</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/fqri8wkee9od1</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1femxrr</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>I definitely need more linear holos</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1femxrr</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1felsm0</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>Trouble with Orly.</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1felsm0/trouble_with_orly/</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1felavd</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>first of all…I have a problem🫣 secondly, dollar tree haul 😁</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1felavd</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1fekf0x</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>can’t stop staring at my nails… DVN - Nostalgia</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/96n19yegq8od1</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1fekea8</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>Tips on growing and keeping nails long?</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fekea8/tips_on_growing_and_keeping_nails_long/</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1fekbht</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Looking for an iridescent flake top coat gel.  </t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fekbht</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1fek9fa</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>I need nail advice, bc I kinda hate these!</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tt8fhlxap8od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1fek77p</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>Clionadh appreciation post</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dynkr8euo8od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1fejpw1</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>my first "special" polish -- obsessed! (poparazzi glass ceiling)</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fejpw1</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1fejcje</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>Polish Me Silly See Me Glow color</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/496p6fqhi8od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1fej3w2</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>Recent Haul Comparisons</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fej3w2</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1feir2b</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>Cottagecore nails 🍂</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1feir2b</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1feia3d</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cirque's Bisou Bisou dupe? </t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1feia3d/cirques_bisou_bisou_dupe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1fehryf</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>Cuticle nippers</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fehryf/cuticle_nippers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1fehmlg</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>The Phoenix Queen</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fehmlg</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1fegwy8</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>It’s intended to be a holiday polish, but I think it’s beautiful for autumn!</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r6dkm1sk08od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1fee51r</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>Today I broke my personal record!</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fee51r/today_i_broke_my_personal_record/</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1fedowh</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>First ILNP order!</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6tknob09d7od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1feddoq</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>First success with magnetic! Love how it shines in direct sunlight (halfway in vid)</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hj0vp6qwa7od1</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1fed6ls</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What are the white lines on my nails? </t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fed6ls</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1fecsf1</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A happy surprise </t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0obmaj2m67od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1fecqsw</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>Doing My Part to Inform People about Gel Allergies</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fecqsw/doing_my_part_to_inform_people_about_gel_allergies/</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1fecgay</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Forest sunset inspired nails </t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x727qeh647od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1fec977</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Looking for gel polish recs </t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/030zttjs27od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1febzhz</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>ILNP Vineyard 🍇</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1febzhz</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1febox4</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>Subtle Glitter Mani</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6fwx40ohy6od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1febnp3</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>'No Time on a Sunday' Dark Pink</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/qR6wjWm</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1febfuh</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>Great Lakes Lacquer</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1febfuh</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1febaxb</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>Help, it’s so beautiful I don’t know what to do with myself</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1febaxb</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1feaq8s</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Deep Space from ILNP is so freaking pretty </t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1feaq8s</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1fe9wq5</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I'm in love 💕 with this polish 💅. </t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/89xr12slk6od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1fe9ay0</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>Beaux Rêves - Light My Fire 🕯️</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fe9ay0</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1fe99on</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>gonna join the 'vaguely autumnal skittle' club</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fe99on</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1fe97vc</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>Gorgeous in any lighting!</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fe97vc</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1fe8ir4</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What I wanted vs what I got </t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fe8ir4</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1fe7qiu</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Final Siren Song of the Summer </t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fe7qiu</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1fe79cf</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How do I deal with peeling UV gel nail polish? </t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fe79cf/how_do_i_deal_with_peeling_uv_gel_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1fe5zwm</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>Is there any savings these (I need them to last until the 23rd) or do I have to start over?</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fe5zwm</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1fe5z4f</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>ILNP - Pink Lemonade</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fe5z4f</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1fdoptn</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>Biab with mylee</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fdoptn/biab_with_mylee/</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1fewcve</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>chucky inspired nail art by me😊</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vshb4l8ctbod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1fevtoo</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Throwback to the first set I ever did 😮 </t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fevtoo</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1fevgxd</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>Bob's Burgers x Beetlejuice 🪲🧃</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fevgxd</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1feu8x6</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>Going back to school: Striping tape nail art was so satisfying😭</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l32pxyg84bod1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1feu0t8</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>Hey girls, I made this design for Halloween a year ago, should I use it again or change some details?</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yk9ld5mt1bod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1fess9i</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>Picked up a new hobby in June….here’s all my sets so far, just for me!</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fess9i</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1feshfu</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>im trying to make my press-ons stronger, what can i do after finishing a set?</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1feshfu/im_trying_to_make_my_pressons_stronger_what_can_i/</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1fesdcd</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My spooky new set! </t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fesdcd</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1ferarh</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>Brush and product recommendations for detailed art with lacquer polish?</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ferarh</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1feo8s4</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t xml:space="preserve">is it okay if i forgot my base coat? </t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1feo8s4/is_it_okay_if_i_forgot_my_base_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1fenwpf</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>Beetlejuice nails I did on my bestfriend for the movie!! Also the longest nail extensions ive ever done 😭🪲🧃</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/nbi15x5ph9od1</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1fentxa</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>ACOTAR inspired press ons I made 🦇🫶🏼</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fentxa</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1felvv2</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>Girlies is this to childish or?</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rs8qny1k19od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1fek6kw</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t xml:space="preserve">GUYSSS I finally had it happen </t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fek6kw</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1fej065</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>first gel x set done by me on myself</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fej065</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1fei3vt</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>Rainy set for fall</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/soui730f98od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1fehu3k</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>Autumn gnome set</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fehu3k</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1fehe1f</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>Opinions</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gjbxh0b348od1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1fegjcg</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>💧 summer nails</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fegjcg</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1feg1pt</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hello! These nails were made for me by my friend Desiree, do you like the color pink? </t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1feg1pt</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1fef4vs</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>Loving the cat eye gels recently!</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/acncmc7on7od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1feeqhd</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>Girlssss, one or two?</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1feeqhd</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1feba27</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>Practicing painting ft. lilac nails &lt;3</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mhspwe1ev6od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1feaees</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>Tips 4 starting making press ons?</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1feaees/tips_4_starting_making_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1fe8s8l</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Favourite set I’ve ever done </t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fe8s8l</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1fe5uu2</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>Foil work fun</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fe5uu2</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1fe5a5j</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Little ghost face set! 👻 </t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qnxzf9vc65od1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1fe4yml</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I’m trying out gel nail polish and gems </t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zkqyfobz15od1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Sep 13 08:09:56 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_09_15.xlsx
+++ b/data/collected_data/2024_09_15.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C822"/>
+  <dimension ref="A1:C989"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14407,6 +14407,2845 @@
         </is>
       </c>
     </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1ffp19h</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>new  nails</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kf9b1cn45jod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1ffocpu</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>Fill appointment tomorrow, do you think they are long enough to reshape to a shortish stiletto?</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g2pkvvadwiod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1ffnfm2</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help identifying these opi minis </t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m7t8j5onkiod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1ffmmxp</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How would you ask for this in the nail salon? Inspo: @LEMINIMACARON on instagram </t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mblh5n4qbiod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1ffnchf</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>Tried a new shade but I don't like it much (gel nails)</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ffnchf</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1ffn692</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>Recommendations for weak press on glue (Read Description)</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ffn692/recommendations_for_weak_press_on_glue_read/</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1ffm4x0</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>Nail Extensions??</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ffm4x0/nail_extensions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1fflj80</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>Various nail colors and lengths (hard gel)</t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fflj80</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1ffly9z</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Played dress up today </t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6c12wswl4iod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1fflvpr</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>Vampiric red</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fflvpr</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1ffluxr</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time using magnetic polish and I’m in love </t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ffluxr</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1ffltvd</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>Nude nails for Job interviews coming up</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6belrtaf3iod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1ffld6a</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>First timer</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ffld6a/first_timer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1fflcsp</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>Mickey ghost nails 👻</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fflcsp</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1fflazt</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>Cake Day Ombré Nails</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fflazt</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1ffl2f5</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>Hazbin Hotel set 😍 my nail tech ATE</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sso1v95qvhod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1ffkohn</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>My nail pet peeve, am I being too picky?</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rssjt9hzrhod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1ffkamb</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>I guess the shark at least ate, but as a whole, this did not eat. 😂</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ffkamb</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1ffirb8</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>Stupid question: how do you call this kind of fake nails?</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ffirb8</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1ffk43l</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>Slightly more interesting French tip</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ffk43l</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1ffjo2t</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>Pretty cool</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lexuwpmmihod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1ffj74a</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>Getting ready for fall! This color is called peach cider 🍑</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tzbqrri9ehod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1ffj721</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>Something Spooky</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mngk3k7aehod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1ffiwlk</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>Getting into spooky season!</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ffiwlk</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1ffiiu3</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First set in over a decade </t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5cbze4t28hod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1ffhq3k</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t xml:space="preserve">After so many services, a little rest </t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c9i2nwyt0hod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1ffhpm2</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>Birthday set🌸</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ffhpm2</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1ffhcql</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>my go-to color!!</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pbhi8c2gxgod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1ffh73x</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>3week Removal</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ffh73x/3week_removal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1ffh5n7</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>Pallet cleanser nails</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aexdankpvgod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1ffh5h5</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My nail person always does me right </t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6q2o4b5ovgod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1ffgw9q</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>I'm blue da ba dee da ba da~</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uu5wqqbetgod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1ffgqdx</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>Teal and Gold Chrome with Gems</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ffgqdx</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1ffgnhv</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>Walk me through it?</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ffgnhv/walk_me_through_it/</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1ffgibj</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Very demure, very cutesy </t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fdhbsimypgod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1ffgdyy</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A promise made in 2020, a promise kept. </t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ffgdyy</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1ffgbtd</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>Nail day check in 💅🏼🩵🫰</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ffgbtd</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1ffg23n</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>Scarab/Beetlejuice nails 😍</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ffg23n</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1fffsvj</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t xml:space="preserve">april - now 👀 </t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6sn4b201kgod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1ffezai</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>Glitter ombré nails</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qf2xdmc6dgod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1ffexfo</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>Nail tech peeled off hard gel</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nsku1u3rcgod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1ffeikl</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t xml:space="preserve">nails as a work of art </t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5mg663ad9god1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1ffcdgp</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>Primers/bonders help please!</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ffcdgp/primersbonders_help_please/</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1ffeapw</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How much is it worth? </t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ffeapw</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1ffe9fm</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>3rd time doing my own nails, how’d I do?</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ffe9fm/3rd_time_doing_my_own_nails_howd_i_do/</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1ffe6pj</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>Holding on to summer with these ones</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3q4xskfp6god1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1ffe69y</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>You like? 🖤</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/byyi8w8m6god1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1ffdnd2</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>My nail tech knocked it out of the park 🤩✨🌈</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h14q959k2god1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1ffdjf1</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>Stick on nail brands</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ffdjf1/stick_on_nail_brands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1ffd6ta</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>First ever set of acrylics!</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ffd6ta</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1ffczvp</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>An old design I did</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xjsljhtmxfod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1ffcpz8</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>Advice on nail color for my girl</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ffcpz8/advice_on_nail_color_for_my_girl/</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1ffce1a</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>Halloween Nails</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/tjr9wz44tfod1</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1ffcars</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>nail advice</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ffcars/nail_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1ffcag6</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What’s the most common cutting corners/sloppy work  issue you’ve seen on nails lately? </t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ffcag6/whats_the_most_common_cutting_cornerssloppy_work/</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1ffca7n</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>builder gel trouble?</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ffca7n/builder_gel_trouble/</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1ffbuyq</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>chrome moment 🤍🦢</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n8r63br6pfod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1ffbu62</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gel Kit </t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ffbu62/gel_kit/</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1ffbti2</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>what shape would suit my natural nails best?</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ffbti2</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1ffb1ig</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>What nail shape would go with my fingers</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ffb1ig</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1ffau41</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Let my boyfriend pick the colors </t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ffau41</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1ffaok8</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>What do you think?</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3vivxvp8gfod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1ffanvz</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>Dark Horse</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lssye8l5gfod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1ffa9v1</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>Velvet nails</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ffa9v1</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1ffad5m</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>RIP, Little Guy 😩</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ffad5m</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1ffa741</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>🩶 Lemming Lacquer Samhainophobia 🧡 Funky fall flakies 👻🎃</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ffa741</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1ffa1lv</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New to Nails- any advice for brittle nails? </t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ffa1lv</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1ff9yxq</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t xml:space="preserve">which uv lamps are good? </t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ff9yxq/which_uv_lamps_are_good/</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1ff9xto</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>My sis fulfilled my whimsical dreams 🖌️🎨🍄</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eqb4puvsafod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1ff9sq1</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>Dip + Gel?</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ff9sq1/dip_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1ff9v3x</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2 patterns + clean cut by diamonds </t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nzgwzrh9afod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1ff9to2</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Changing it up with short square </t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7rlqm62z9fod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1ff9q2c</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>What nail shape would look best for my hands?</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ff9q2c</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1ff9bre</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>soft builder/gel polish chipping?</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nljirm1b6fod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1ff962c</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>First fall feels set of the season (yes I know it isn’t technically fall yet but I love fall)</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ff962c</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1ff8rh5</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>One of my favorite sets in a long time :)</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vtog7dd62fod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1ff81e1</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Time for wine </t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ff81e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1ff7spj</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>Love this blue polish 🥰</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ff7spj</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1ff7f84</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The day was September 12, it was a crisp 74 degrees in Tennessee. You know what that means…. </t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bj86zsj9seod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1ff7cab</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>once you go russian you NEVER go back</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ff7cab/once_you_go_russian_you_never_go_back/</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1ff79jy</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>What did i do to deserve this</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4uy5isu3reod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1ff6w9p</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>I’d give this a 7/10</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uredi1adoeod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1ff6o6v</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>First time with a dip mani</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ff6o6v</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1ff6hzv</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>What are these nails?/how would you tell your nail tech what you want? Inspo from nailzkatkat on TikTok</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z325edffleod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1ff2io9</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Messaging nail tech about a design idea, is it weird? is it rude? </t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ff2io9/messaging_nail_tech_about_a_design_idea_is_it/</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1fexms3</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>My charms turn pink or the shine wears off despite sealing with top coat?</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fexms3</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1ff604w</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Got Almond for the First Time! </t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kw11wb2rheod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1ff55jj</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>Am I being too picky?</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ff55jj</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1ff4uy8</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>What do you think?</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ff4uy8</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1ff4gxt</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>From square to ballerina for fall season, what do you think? 💅🏼</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t61t05x76eod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1ff3ztj</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>I’m a nail artist . What do you think?</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ff3ztj</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1ff3yom</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>Fall set</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f2rccnlc2eod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1ff3s3s</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>my fav nail colour 🩸🦇</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vi5w6yby0eod1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1ff2nvs</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gel nail advice </t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ff2nvs/gel_nail_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1ff24vu</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Impressed by this ILNP polish. </t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ff24vu</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1ff1pr5</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I didn't know the bane of my existence would be this type of gel extension (paid a lot, saved for some time for it and now I'm grieving) </t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ff1pr5</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1ff15k4</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A true travesty </t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/66hh2skvedod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1ff0pea</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>My nail tech is amazing !!</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ff0pea</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1ff0l14</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The process of my nails. Do you like it this long? </t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ff0l14</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1ff0g9m</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>My End of Summer Set</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5to8my088dod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1ffpgu7</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phoenix Polish and ILNP </t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ffpgu7</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1ffog9u</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>I’m tired of stained nails but scared of doing at home gel-x</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ffog9u/im_tired_of_stained_nails_but_scared_of_doing_at/</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1ffo71x</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>First(?) full self-mani :P</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ffo71x</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1ffn4vs</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>OPI repair mode vs Nailtiques Formula 2 Plus</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ffn4vs/opi_repair_mode_vs_nailtiques_formula_2_plus/</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1ffltzx</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time using magnetic polish and I’m in love </t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ffltzx</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1fflkbo</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>Beginner La(c)querista</t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0b1t2xkq0iod1</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1ffkudb</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t xml:space="preserve">🐑 🧶 LynBDesigns Wooly </t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ffkudb</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1ffkt6y</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>Anyone else obsessed with changing their nail polish every couple of days?</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ffkt6y</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1ffkns1</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>Need opinions.</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ffkns1</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1ffkiqi</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>Holo Taco</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ffkiqi/holo_taco/</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1ffhrkb</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Different lighting what I like to call cement purple. </t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ffhrkb</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1ffg8j5</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>I've been using painting my nails as a way to help my OCD and negative thoughts.</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/506w8h0ongod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1ffg438</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>ILNP Starlight</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ffg438</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1fffsh7</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>Which top coat for my situation?</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fffsh7/which_top_coat_for_my_situation/</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1fffatc</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>I almost didn’t buy this!</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fffatc</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1ffegyo</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>Nail polish popping off without using peel off base coat?</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ffegyo/nail_polish_popping_off_without_using_peel_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1ffefsa</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>Mermaid Bait is the shiftiest polish!</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ffefsa</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1ffe2y9</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Collection picture and Questions </t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ffe2y9</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1ffdf6x</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>jade quartz nail art</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ffdf6x</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1ffdasz</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>Dazzle Dry and Acrylate Allergies</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ffdasz/dazzle_dry_and_acrylate_allergies/</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1ffcxit</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>🧿 Ethereal Creature 🦋 by Ethereal Lacquer</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/70cp3e05xfod1</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1ffcqzr</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>Anyone else always fighting the urge to add glitter? 😅</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/re6zgfzsvfod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1ffc1i9</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>Really proud of this one!</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3k3mby3iqfod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1ffbs0z</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>First time posting here, hi!</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ffbs0z</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1ffbh2h</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>Speedy Velvet!</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ffbh2h</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1ffbanu</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>Trying out square shorties this fall</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6mvyp2wxkfod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1ffa53j</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>🩶 Lemming Lacquer Samhainophobia 🧡 Funky fall flakies 👻🎃</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ffa53j</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1ff9hny</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What are your favorite polish combos to wear together? </t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ff9hny/what_are_your_favorite_polish_combos_to_wear/</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1ff8cwl</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>Wedding nails</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6hmowo27zeod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1ff7pup</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>WFL Tweetie Pie - Yellow polish of my dreams ✨🫶</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ff7pup</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1ff77rz</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>You lot influenced me to get a horseshoe magnet and... I can't. It's too pretty 🥺</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/k0zlpjwiqeod1</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1ff6wu5</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Stamping plate question? </t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ff6wu5/stamping_plate_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1ff6vs8</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I don’t normally do my nails, please humor me. </t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tlb42yw9oeod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1ff65ep</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>What brands are dropping tomorrow?</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ff65ep/what_brands_are_dropping_tomorrow/</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1ff5iww</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>Fall is here 🍂🍁</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ff5iww</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1ff5366</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t xml:space="preserve">what happened? </t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ztfv8udxaeod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1ff51yo</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>Rockstar Y2K nails!</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ff51yo</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1ff4rsw</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t xml:space="preserve">🍂 It's finally fall! 🍃 Lost in the Woods &amp; Misery </t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ff4rsw</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1ff4fkj</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>Beginner trying out cute designs these are my lemon nails🍋</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8riijvay5eod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1ff4d3i</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>For my fellow Purple Lovers™️</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ff4d3i</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1ff41gm</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>My first Death Valley order. How did I do?</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n711ywqs2eod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1ff3zlo</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What’s your favorite non quick dry top coat? </t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ff3zlo/whats_your_favorite_non_quick_dry_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1ff3yy3</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>Maker/owner PR: A little yellow...</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y1cb1y1t1eod1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1ff2t74</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>💚🩵Nail Frens Gradient🩵💙</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ff2t74</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1ff2s1u</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>Powerpuff Girls 💚🩷💙</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ff2s1u</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1ff1xhk</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>I don't normally choose my polish colors based on the season, but fall is in the air and burgundy feels so right!</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2hbshq6yldod1</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1ff18x6</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>Day 1 vs day 15</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ff18x6</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1ff0rxp</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t xml:space="preserve">You, of Unshakable Conviction </t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ff0rxp</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1fey0me</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>Blue Shorties</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/jaezCe0</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1fexxte</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>Jfc I was just grabbing a dress.</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fexxte</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1fflwu5</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time using magnetic polish and I’m in love </t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fflwu5</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1ffk95p</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>Complete fail, but I have a shark nail now. 😂</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ffk95p</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1fff2e4</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>One of the most fun + easy designs is a glitter ombré.</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ddvjlfsudgod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1ffe6k5</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First manicure in awhile </t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ffe6k5</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1ffe2gv</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>New at this</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ffe2gv</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1ffbzmq</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>Oriental art</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ffbzmq</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1ffag28</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>blu set</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ffag28</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1ff95q9</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>Hello people, today I did these nails, they are one of the first ones I do, what do you think? 💕(OC)</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/12pw6h325fod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1ff8xp3</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>Did this set on my sister in law for her wedding ;)</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/la008c3e3fod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1ff8j8f</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>Last weeks orders ✨</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ff8j8f</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1ff8fsj</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>French with chrome</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ff8fsj</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1ff8b45</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>Another watercolor set 💅🏼✨️</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ff8b45</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1ff7x2l</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>All Hail The Pumpkin King</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1ff7x2l/all_hail_the_pumpkin_king/</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1ff3n3b</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>My take on Enchanted Forest 🧚🏾‍♀️🌱</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ff3n3b</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1ff32vi</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>Press On Vault</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j2d186zgvdod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1ff2lyv</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>Gel nail allergy— alternate options &amp; caution!!</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1ff2lyv/gel_nail_allergy_alternate_options_caution/</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1feziuu</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>It's spooky season! This is just my warm up set! 🍁</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5id3znwdycod1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Sep 14 08:09:51 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_09_15.xlsx
+++ b/data/collected_data/2024_09_15.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C989"/>
+  <dimension ref="A1:C1166"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17246,6 +17246,3015 @@
         </is>
       </c>
     </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1fggxm0</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>first diy press ons!</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fggxm0</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1fggplx</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Bits and Bobs </t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xs970l1f8qod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1fggobt</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>Nails nails nails love them all ❤️</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fggobt</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1fggim4</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>Looking for a black gel polish that is as black as possible</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l825tgot5qod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1fgg60c</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>do you guys think i should change the fourth nail to something else?</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z5g6j1pj1qod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1fgg0z7</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>My first ever long set</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fgg0z7</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1fgesc5</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>Can I use soft gel on top of hard gel?</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fgesc5/can_i_use_soft_gel_on_top_of_hard_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1fgfsu5</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What do you think of my nails? </t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wspxlbe0xpod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1fgedqt</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time doing 3D designs </t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fgedqt</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1fge3m3</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>Can’t believe she did this w/ my natural nails. So in love 🍂🍁🍄</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fge3m3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1fgdeb5</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>My nail tech probably missed on this one ☹️</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6n1n0rxd4pod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1fgbi26</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>Natural Nail Overlay</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fgbi26</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1fgd83y</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>Very natural and pretty. What do you think? Do you like them?</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wj8hr01x2pod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1fgckvo</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>Black is so classy</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xoezthkbwood1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1fgcjal</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>Airbrush issues</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fgcjal/airbrush_issues/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1fgbyof</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My first time getting loose glitter </t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/twnzcm65qood1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1fgbyab</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dual Form Polygel Question </t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fgbyab/dual_form_polygel_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1fgby8v</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>Short nails?</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l0nxgpr0qood1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1fgbeor</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>I'm getting a lil too good at gel x 🦋</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5d7c9fakkood1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1fgavu3</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Girls I fell in love with this design </t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r2q3dpmifood1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1fgaurw</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Moody Blue for September </t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wp26t899food1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1fgapq5</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>DIY Autumn Vibe Nails</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fgapq5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1fgamov</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>Soft gel nails 🪻</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fgamov</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1fgafz1</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>Gold with Chrome. Not what I expected!</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fgafz1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1fg9xi3</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I feel suffocated? </t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fg9xi3/i_feel_suffocated/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1fg9pqc</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>Went a little out of my comfort zone with this color</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ec5dakvx4ood1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1fg9lgv</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nude with a little ✨ - press ons </t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w44so1gv3ood1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1fg9f5b</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What black nail polish to recommend </t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8unvu3d92ood1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1fg8vfx</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>Silicon for ombre? Sustainable alternatives for blending polish</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q8vpmarexnod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1fg8uqj</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>Tipping</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fg8uqj/tipping/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1fg8ts8</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>Not perfect, but I love them</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gej6vyezwnod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1fg8m8y</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>What vibe do these give? I'm loving pastels recently</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6trkivp6vnod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1fg7y0f</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>:)</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w7bvny5ipnod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1fg7w9u</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>Whats the best method for nail extensions?</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fg7w9u/whats_the_best_method_for_nail_extensions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1fg7v3g</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>Vegas nailsssss</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fg7v3g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1fg7n24</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Loving my fall set </t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w5v86gvwmnod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1fg7dzb</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>Trying out some cute press ons</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8b7epdrsknod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1fg6t20</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>Love that color</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8qa6k3exfnod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1fg6gh3</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A little mix &amp; match for fall </t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v0yoxnr7dnod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1fg5tdz</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fruit nail art </t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fg5tdz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1fg5rog</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>Can I use builder gel as glue for tips?</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fg5rog/can_i_use_builder_gel_as_glue_for_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1fg5n1f</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>First ever time painting nails</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fg5n1f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1fg5cgx</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>The first set I’ve done on myself that isn’t horrible!</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fg5cgx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1fg4s3y</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>How can I fix the area around my cuticles?</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ti7fa7ba0nod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1fg4ifu</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>Multi-colored fun!</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z4zswd37ymod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1fg4gqu</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Beetlejuice, Beetlejuice, BEETLEJUICE </t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/go1pek8vxmod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1fg46cj</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>My Nailbeds are HUGE **(Toenails)** Help me find adequate press-ons please?🥺🙏🏾</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fg46cj/my_nailbeds_are_huge_toenails_help_me_find/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1fg3y06</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>Really proud of the progress I made doing my own nails</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fg3y06</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1fg412h</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Update from yesterday </t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fg412h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1fg3zn6</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New fall nails </t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fg3zn6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1fg2ysr</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Uv light gel polish </t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cn2ageuemmod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1fg25sy</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>Autumn-coded nails!</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fg25sy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1fg18fj</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>do you prefer acrylic or naturally long?</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fg18fj/do_you_prefer_acrylic_or_naturally_long/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1fg00b6</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>got my wedding nails done:)</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fg00b6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1ffzwaw</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>Blue victorian set</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ffzwaw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1ffzjc9</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>New💜 cute✨</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ukwarqxkwlod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1ffz0nd</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>My wedding babies for tomorrow. Enjoy the claw bcs my fingers are chubby.</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ffz0nd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1ffyjm4</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>Help - growing my nails and choosing the right products?!</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/56wxav20plod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1ffxuc8</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>Never have I ever had chrome</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ffxuc8/never_have_i_ever_had_chrome/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1ffwqdy</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>Alternate to electric nail buffing?</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ffwqdy/alternate_to_electric_nail_buffing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1ffyjb0</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>beetlejuice waterslide nails</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ffyjb0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1ffy5nx</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>yay. 🍁✨</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y5dbw587mlod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1ffxjpe</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail glue or acrylic? </t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ffxjpe/nail_glue_or_acrylic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1ffx5xi</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>This weeks set &amp; I also got my toes done in black  to sort of match🥹</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jdjwljjvelod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1ffwqk4</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>Love press-ons</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/r9bk6mfpblod1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1ffwmc1</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>Cat eye berry nails 💅</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/p5w8vebralod1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1ffwdr9</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>Need Help</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ffwdr9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1ffvk05</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>Decal water slides</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ffvk05/decal_water_slides/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1ffv6nm</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ready for the Season! </t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ffv6nm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1ffv50q</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>Black polish and golden nail stickers ✨🌛</t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ijkxoughzkod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1ffupp6</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>Free set of gel nails - weird to tip with card?</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ffupp6/free_set_of_gel_nails_weird_to_tip_with_card/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1ffuepl</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>Love my Autumn Set</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4avseezhtkod1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1ffucxv</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>Do I need to go to the salon?</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j31xqmy2tkod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1ffubaa</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>Unhas feitas</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s9pda7moskod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1ffu3qk</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>Acrylic vs gel</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ffu3qk/acrylic_vs_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1fftpou</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>My first cat eye on my nails.</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3m5zu7clnkod1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1fftaqm</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>Vampy Red Cat eye nails</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rdtfeyntjkod1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1fft0ht</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>La delicadeza de esta semana 🎀</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l9fsnq84hkod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1ffstow</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t xml:space="preserve">In love with my new autumn nails 🍂 </t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6x5pb2lefkod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1ffsrew</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t xml:space="preserve">He is a good boy and background </t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ffsrew</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1ffsouw</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>First time having my nails done!</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ffsouw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1ffqh11</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>How much are these worth?☺️</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ffqh11</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1ffq40t</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>Terrazzo nails are a trend here in Korea this fall. I’m curious about trends in other countries!</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ppyfsn6tjjod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1ffprfp</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>fresh new set today !!!</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ffprfp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1ffmm7s</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>Sabrina Carpenter MTV VMAs Inspired Nails</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ffmm7s/sabrina_carpenter_mtv_vmas_inspired_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1fggf74</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>Looking for a black gel polish that is as black as possible</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mfjslrlm4qod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1fgg144</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>It’s here! Clionadh Cosmetics haul</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fgg144</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1fgfj5m</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>I got to watch two wonderful family friends get married today. The entire day was amazing. And this is how I matched my nails to my dress!</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fgfj5m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1fgffdc</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>Even in crappy low light, mystic moonstone is a stunner</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fgffdc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1fgeynw</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>Been waiting till fall for this one!</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fgeynw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1fgeei8</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>Gabriel?</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fgeei8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1fgdesk</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>Very demure, very mindful</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fgdesk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1fgd94g</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t>Nutrafol &amp; Kerasal Saved My Nails</t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fgd94g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1fgd29u</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>New subreddit for fans of Lurid Lacquer!</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fgd29u/new_subreddit_for_fans_of_lurid_lacquer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1fgcozd</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Does anyone have Opi Take a Vow, Put it in Neutral, It’s a Girl and Essie Sugar Daddy? </t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fgcozd/does_anyone_have_opi_take_a_vow_put_it_in_neutral/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1fgc0p9</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>I love reflective glitter!!</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fgc0p9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1fgao2h</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>Sand Viper + Fool’s Gold Mooncat dupes?</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qw8ibt3jdood1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1fg9stl</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>I ruined my nails like 4 months ago by buffing them and they still haven't outgrown the damage?</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fg9stl/i_ruined_my_nails_like_4_months_ago_by_buffing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1fg9abm</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>Had my first break, but fixed it thanks to y'all!</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fg9abm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1fg8yl7</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>Tfw you rediscover a polish you used to love 🥰</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fg8yl7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1fg8g9z</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Psilocybin by Clionadh Cosmetics </t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1w5ex5iqtnod1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1fg89r1</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>I need fall to show up faster</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fg89r1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1fg861l</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>Psych Minerals , you’ve impressed me for the millionth time! This polish is the cure for anyone with a broken nail 😂she will make you FORGET</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fg861l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1fg84y6</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Has anyone tried Drunk Fairy Polish? </t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fg84y6/has_anyone_tried_drunk_fairy_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1fg847q</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This is my collection so far (plus my swatchings) </t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fg847q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1fg83a8</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>Can never go wrong with red ❤️</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ternbnrpqnod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1fg80yr</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>Swatch request for ILNP Showstopper and Mooncat Spaceoddity</t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fg80yr/swatch_request_for_ilnp_showstopper_and_mooncat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1fg7xfn</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>Kathleen &amp; Co Camp Crystal Lake</t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zoh3cvlcpnod1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1fg7r43</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t>ILNP Roulette</t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fg7r43</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1fg7pat</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fall, but sparkly </t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fg7pat</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1fg7lgb</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>Looking for dupes similar to Natasha Richardson’s manicure in The Parent Trap.</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/58kg5bujmnod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1fg6h8y</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>Loving this color! 👽</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uxsmxjgddnod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1fg6bcw</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My fav :’)) </t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fg6bcw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1fg5sly</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>Oh now THIS is a good blue glitter..</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fg5sly</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1fg5k0k</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>ILNP: Rosewater</t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fg5k0k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1fg5j5v</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>Painted Polish - All About That Baste</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fg5j5v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1fg4t1c</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How can I fix this? </t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6ec70qeh0nod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1fg41rh</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>Okay, Cadillacquer</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/yy8ubrgnumod1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1fg41ah</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New fall nails </t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fg41ah</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1fg3tso</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>First Death Valley Order!! How to Start?</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fg3tso</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1fg2uon</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Spot the difference! </t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/92lg7evilmod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1fg2trc</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>Fun With Sparkles!</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vwzqi6tblmod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1fg2lx6</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t>Anyone else have polishes that were initially disappointing but you’ve learned to love?</t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fg2lx6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1fg2056</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>Best polish for overcast cloudy weather?</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fg2056/best_polish_for_overcast_cloudy_weather/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1fg1xp3</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>ILNP Someday and Seaside</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g8asjdajemod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1fg1c0t</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Matte for a change </t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jyxopj21amod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1fg11w5</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>🍯Oh Honey🍯</t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fg11w5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1fg0gry</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>Raiders Nail #3 - I did it! ILNP Colors</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fg0bvn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1fg00t2</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>Nailtiques is helping my nails but I can’t apply color on top without it melting</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fg00t2/nailtiques_is_helping_my_nails_but_i_cant_apply/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1ffzoaf</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>It's only going to be 101° today! Downright cool 💗</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ffzoaf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1ffz93x</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>Dr. No &amp; Athymy 💜</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/23igekzgulod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1ffz0cf</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>Which of these products is making my nails peel?</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ffz0cf/which_of_these_products_is_making_my_nails_peel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1ffyskx</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>My first time trying a thermal in many years!</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ko648a0xqlod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1ffyedb</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>Quick dry and glossy top coat?</t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ffyedb/quick_dry_and_glossy_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1ffy21z</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>Does anyone know a good dupe for Rosewater jelly from cirque colors?</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ffy21z/does_anyone_know_a_good_dupe_for_rosewater_jelly/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1ffxqkw</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>The first fall mani 🍂🍁</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mqb2vnb2jlod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1ffxjt2</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>LynB thermals are awesome!</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ffxjt2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1ffx9c3</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The glow of Macchiato Cloud </t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ffx9c3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1ffx87f</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>Mood</t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rj2zh39cflod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>1ffwxz8</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>Silent Library is perfect for Fall</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ffwxz8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>1ffwx0x</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>Just The Coolest</t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ffwx0x/just_the_coolest/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>1ffwibd</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>Do these count as fall nails? 🤔</t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iubqf6iz9lod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>1ffwd2y</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>Leaning into darker polishes lately !!</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zckhynqv8lod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>1ffw1p5</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>Fall nails 🍂🍁</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ffw1p5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>1ffw00t</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>Can I join the club??</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ore2w7e36lod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>1ffvh3m</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>yay. 🍁</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/itvaxs732lod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>1ffvelw</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>Haalllp! Please. With this Lurid Lacquer wishlist.</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ffvelw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>1fftqna</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>Emily de Molly shifty extravaganza</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fftqna</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>1fftqim</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>Delivery from Prism Polish just arrived</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fftqim</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>1fft8yl</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>Clionadh Haul - SO Excited!</t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/683jet8cjkod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>1ffsbwp</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tyler’s Trinkets “Needy B*tch Blue.” Cute backstory behind the name in comments. </t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ffsbwp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>1ffrk40</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>A thank you to the community</t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ffrk40</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>1ffrep6</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Qdtc alternatives from very mainstream brands? </t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ffrep6/qdtc_alternatives_from_very_mainstream_brands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>1ffrei4</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Opinions on this colour? </t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ktztva4a0kod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>1ffqbqk</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Thermal French </t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ffqbqk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>1ffq0id</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>I guess I’ve been in the mood for pinks and purples</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ffq0id</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>1fggvrt</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t xml:space="preserve">polygel/blunt ash monster claws </t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fggvrt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>1fggq0h</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Foils Here they are on </t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fggq0h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>1fgfsc0</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Design by CB NAILS 💅 </t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vmi0r0duwpod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>1fgctxk</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>First time doing press on</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fgctxk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>1fgcc9i</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t>The nails from my favorite movie, who guesses what it's called? 🙊</t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vqkv1lmxtood1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>1fgcb9v</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>Other Halloween nails I did today! What do you think of these? 👻</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t2pbp7fntood1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>1fgc7ra</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail art help! </t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1fgc7ra/nail_art_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>1fgbobr</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mickey nails </t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a384lj39nood1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>1fgbnvg</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Reddit Nails </t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/p/C_n-q3bP67D/?igsh=eHFua3NoenR1OWQz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>1fgb9m1</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t>First time</t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fgb9m1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>1fg75n8</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>Friday the 13th</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fg75n8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>1fg6rmn</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>What do you think of these nails I did today? Halloween vibes are starting to be felt ✨🎃</t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y5al2gjnfnod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>1fg5nl6</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t>Spirited away 💨</t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fg5nl6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>1fg4wb0</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Junk nail set I did on myself </t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fg4wb0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>1fg2k9q</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>Decals great fun to work with</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fg2k9q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>1fg2d14</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Foil fun </t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fg2d14</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>1fg006q</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>Blue victorian set</t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fg006q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>1ffwzkm</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t>Who’s up for a little spooky vibe for Halloween? But this set is just too cute!</t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qg01mp1ddlod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>1ffth2t</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Friday the 13th nail art </t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ffth2t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>1ffpz2o</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>Teal and Dark Gold Chrome</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ffpz2o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>1ffppuc</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ladybirds </t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ffppuc</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Sep 15 08:09:08 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_09_15.xlsx
+++ b/data/collected_data/2024_09_15.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1166"/>
+  <dimension ref="A1:C1342"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -20255,6 +20255,2998 @@
         </is>
       </c>
     </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>1fh7j7p</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t>Had to cut my nails, which I had been growing for 4 months..</t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fh7j7p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>1fh4syz</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>Can anyone help me find this shade name? or a gel polish like it?</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/epiomp8mmwod1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>1fh67fa</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t>Told this colour is too yellow for me?</t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w69ey5cj3xod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>1fh5xy5</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t>Halloween 👻</t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fh5xy5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>1fh5xdf</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t>What can I do to improve how it looks/Make it like cleaner?</t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fh5xdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>1fh5svf</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>Still deciding on the perfect wedding manicure ✨✨</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dj4s609nywod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>1fh578r</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t>press ons i made ☺️</t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fh578r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>1fh4p8o</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Shiney </t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/88upgckllwod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>1fh4o83</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t>Fall time nails 💅🏽🍁🍂🧡</t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h3hfrcs9lwod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>1fh4o2v</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t>Is anyone concerned about doing gel long-term? I just got my builder gel nails filled and my fingers are burning</t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fh4o2v/is_anyone_concerned_about_doing_gel_longterm_i/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>1fh4f9o</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t>UV lamps</t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fh4f9o/uv_lamps/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>1fh44us</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t>Fresh nails</t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fh44us</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>1fh3roq</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t>ah shit we gotta go bald (very sad rn)</t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fh3roq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>1fh3n6s</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t xml:space="preserve">fall nails </t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ov1lrxe3awod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>1fh3b4t</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>Love this color 🦎🌿</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7p1edaoo6wod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>1fh3a9p</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What to buy? </t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fh3a9p/what_to_buy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>1fh37bg</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t>rip blue set. time for red n gold</t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fh37bg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>1fh30ss</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t>Need advice ❤️</t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/22v8si0p3wod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>1fh2mcj</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>First ever set of nails but how do y’all do aaaaanything car-wise wit these 😭😭😭 I take like 10x as long to do tasks I could do so easily</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rfeaaa5hzvod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>1fh2e8p</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Which shape suits me best? </t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fh2e8p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>1fh2e4t</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Monarch Lacquer - Freeze Dance </t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fh2e4t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>1fh2dqk</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t>What do you guys think?</t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fh2dqk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>1fh1rrl</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>Today's adventure in attempting 'color' instead of mainly black ~</t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fh1rrl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>1fh2a7b</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>A dumb question about nail oil.</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fh2a7b/a_dumb_question_about_nail_oil/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>1fh1zn4</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t>Is this normal?</t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fh1zn4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>1fh1hj0</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>Questions regarding peeling nails</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fh1hj0/questions_regarding_peeling_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>1fh10jh</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t>Nail polish clean out #1</t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ktot2wkfjvod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>1fh0hg3</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>How to ask for what I want??</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ha04tel5evod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>1fh0j8d</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t>Paris Hilton "BBA" Music Video Inspired Nails</t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3d3byc6kevod1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>1fh0ybg</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t>My first attempt at a design 🫣</t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fgsyh3auivod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>1fh0s9u</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t>Spooky season 🕷️</t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gzfmsni0hvod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>1fh0mfd</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t>Whirlypop Love</t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fh0mfd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>1fh0j3s</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Simple but makes me happy 😊 </t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gkqaf5rlevod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>1fh03pj</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Black French tips &gt;&gt;&gt; </t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v1t8tr9lavod1.gif</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>1fgyqv9</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Disney ready nails! My nail tech kills it every time </t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6p2t9gu3yuod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>1fh00kb</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t>Cat eye nails 🫦</t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e11orw4s9vod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>1fgzxvd</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t>Is anyone else completely dependent on builder gel?</t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fgzxvd/is_anyone_else_completely_dependent_on_builder_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>1fgzurh</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t>can you get acrylics if your nails aren’t past your fingertips</t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fgzurh/can_you_get_acrylics_if_your_nails_arent_past/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>1fgzq58</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t>For my glitter girls✨🫶🏼🩷</t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6eboi4cy6vod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>1fgzaux</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t>Best and shinniest top coat?</t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fgzaux/best_and_shinniest_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>1fgyzcv</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t>Holes in builder gel?</t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0b8gwtd70vod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>1fgyymb</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t>I love my girlfriend’s new nails</t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ma4bept00vod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>1fgywt1</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t>How did I do?</t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fi0kqnfkzuod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>1fgystu</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t>Nail Polish brands that have unique and interesting polishes??</t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mfgr7yylyuod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>1fgys25</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t>First time doing my nails! Any tips?</t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3hue5qafyuod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>1fgydr2</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t>New week, new set 😍</t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2sx4boh0vuod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>1fgxzex</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fall nails </t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fgxzex</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>1fgxzc0</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Need help solving a mini-mystery </t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fgxzc0/need_help_solving_a_minimystery/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>1fgxxnn</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t>I just wanted to show my nail progress ever since I stopped biting my nails! :)</t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fgxxnn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>1fgxxc9</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t>Just came by to say my nail tech ATE!!</t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fgxxc9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>1fgxw35</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t>Really love my nails ❤️</t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fgxw35</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>1fgxc6t</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t>I looove this rusty red color! It’s just so perfect for autumn (:</t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m9rcyyy9muod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>1fgvzy8</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Just finished doing my own nails for the 2nd time </t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w3re9saabuod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>1fgvum5</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fresh gel polish mani/pedi ✌️ ☮️ </t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fgvum5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>1fgvsjv</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t xml:space="preserve">delicate , just beautiful . </t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sm2ijdyo9uod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>1fgveom</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First ever professional set </t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/acm7w8tv5uod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>1fgvdnu</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t>What do you think?🌸</t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qu79r55o5uod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>1fgvcvl</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t>Matric dance nails</t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b806898i5uod1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>1fgv7kv</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t xml:space="preserve">peeling nails after staring to use nail polish </t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fgv7kv/peeling_nails_after_staring_to_use_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>1fgv69b</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t>Nude nails and I'm obsessed!</t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fgv69b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>1fgv1p9</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t>Does it look too fake?</t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fgv1p9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>1fguyli</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t>my first ever set! &lt;3</t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fguyli</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>1fguje1</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Recently switched to almond shape </t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fguje1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>1fgub48</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hard Press On Recommendations </t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fgub48/hard_press_on_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>1fgt876</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t>Help with removing Lights Lacquer polish</t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fgt876/help_with_removing_lights_lacquer_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>1fgtc20</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t>does anyone know where i can buy NailsInc in the United States?</t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fgtc20/does_anyone_know_where_i_can_buy_nailsinc_in_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>1fgufww</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t>I’m obsessed with how I did my sister’s nails 😍</t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7g3j4xqyxtod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>1fgu730</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t>New to Home dipping!</t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fgu730</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>1fgu3he</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love a blue nail &lt;33 </t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fgu3he</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>1fgu21x</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New set! Still learning . ݁₊ ⊹ . ݁˖ . ݁ </t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tt4qep4sutod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>1fgtwfc</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t>Pink nails</t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0rqd477ittod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>1fgtu1i</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I tried moon cat for the first time </t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fgtu1i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>1fgtmj4</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t>Nail rehab post-BIAB</t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fgtmj4/nail_rehab_postbiab/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>1fgtkc1</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t>Sonny Angel!</t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9v1h5m6tqtod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>1fgtj4c</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t>What do y’all think of mine (black) and my sisters (red) nails?</t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/45m7qasiqtod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>1fgthi9</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t>Just got some new polish today!💅</t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fgthi9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>1fgtff7</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t>The Portals of Sunflower Grove</t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fgtff7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>1fgt9b5</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t>Mermaid seashell nails 🧜‍♀️🐚✨</t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/885i1unfotod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>1fgt79y</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Does this count as fall? </t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8xxeoepzntod1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>1fgt57c</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t>Roses are red, True love is rare, Booty, booty, booty, booty rockin everywhere</t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fgt57c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>1fgt0eg</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t>White Pearl nails - I feel boring but I have an interview Tuesday so I thought they'd be timeless.</t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/avu68o2rmtod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>1fgsnsg</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t>Happy belated Friday the 13th</t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/93usg0khitod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr">
+        <is>
+          <t>1fgs9zh</t>
+        </is>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t>Have a concert tonight, my nails are ready💅🏼</t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/88mz3ldiftod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr">
+        <is>
+          <t>1fgs7xt</t>
+        </is>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t>In love!</t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/abg4tz02ftod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr">
+        <is>
+          <t>1fgi50z</t>
+        </is>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Are these nails as bad as I think they are? </t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fgi50z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr">
+        <is>
+          <t>1fgrtd4</t>
+        </is>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t>Magnet tutorial vampy cat eye</t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/u4a1z14ubtod1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr">
+        <is>
+          <t>1fgs3at</t>
+        </is>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t>this weeks set!</t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fgs3at</t>
+        </is>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="inlineStr">
+        <is>
+          <t>1fgs2c7</t>
+        </is>
+      </c>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t>I couldn’t decide, so I chose all💅🏽✨</t>
+        </is>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fgs2c7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="inlineStr">
+        <is>
+          <t>1fgrzbr</t>
+        </is>
+      </c>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sage Grey French Tip nails </t>
+        </is>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lj81qgg6dtod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="inlineStr">
+        <is>
+          <t>1fgrlry</t>
+        </is>
+      </c>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t>New nails for the week!</t>
+        </is>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rti5psk4atod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="inlineStr">
+        <is>
+          <t>1fgrg8e</t>
+        </is>
+      </c>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t>What do y’all think?</t>
+        </is>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fgrg8e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="inlineStr">
+        <is>
+          <t>1fgqg78</t>
+        </is>
+      </c>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My new autumn nails </t>
+        </is>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r70zojrq0tod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="inlineStr">
+        <is>
+          <t>1fgqdrp</t>
+        </is>
+      </c>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t>My 10th set and I’m so in love with all the art I did!!</t>
+        </is>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lyezwc080tod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="inlineStr">
+        <is>
+          <t>1fgq7c5</t>
+        </is>
+      </c>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t>Gel polish beginner - need advice from experts</t>
+        </is>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aofe0dzsysod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="inlineStr">
+        <is>
+          <t>1fgpyh0</t>
+        </is>
+      </c>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t>So cute it's scary!</t>
+        </is>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fgpyh0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="inlineStr">
+        <is>
+          <t>1fgpqkm</t>
+        </is>
+      </c>
+      <c r="B1262" t="inlineStr">
+        <is>
+          <t>Advice about nail salons and acrylics, are fillins cheaper?</t>
+        </is>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fgpqkm/advice_about_nail_salons_and_acrylics_are_fillins/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="inlineStr">
+        <is>
+          <t>1fgpqbb</t>
+        </is>
+      </c>
+      <c r="B1263" t="inlineStr">
+        <is>
+          <t>Hello world may I punch you</t>
+        </is>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fgpqbb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="inlineStr">
+        <is>
+          <t>1fgpiyn</t>
+        </is>
+      </c>
+      <c r="B1264" t="inlineStr">
+        <is>
+          <t>My nails, but better?</t>
+        </is>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fgpiyn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" t="inlineStr">
+        <is>
+          <t>1fgpe7k</t>
+        </is>
+      </c>
+      <c r="B1265" t="inlineStr">
+        <is>
+          <t>Dark like my soul but sparkly like my personality. 🤣</t>
+        </is>
+      </c>
+      <c r="C1265" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q71ro1messod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="inlineStr">
+        <is>
+          <t>1fgnq50</t>
+        </is>
+      </c>
+      <c r="B1266" t="inlineStr">
+        <is>
+          <t>Getting fake nails removed</t>
+        </is>
+      </c>
+      <c r="C1266" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fgnq50/getting_fake_nails_removed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="inlineStr">
+        <is>
+          <t>1fh7dvu</t>
+        </is>
+      </c>
+      <c r="B1267" t="inlineStr">
+        <is>
+          <t>Spooky, but make it fun 👻✨</t>
+        </is>
+      </c>
+      <c r="C1267" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fh7dvu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="inlineStr">
+        <is>
+          <t>1fh55el</t>
+        </is>
+      </c>
+      <c r="B1268" t="inlineStr">
+        <is>
+          <t>House of Hades + “Howdy” stickers</t>
+        </is>
+      </c>
+      <c r="C1268" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fh55el</t>
+        </is>
+      </c>
+    </row>
+    <row r="1269">
+      <c r="A1269" t="inlineStr">
+        <is>
+          <t>1fh4cbo</t>
+        </is>
+      </c>
+      <c r="B1269" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Bday nails 🥳 ILNP &amp; Mooncat playing nice together with those shifts!! </t>
+        </is>
+      </c>
+      <c r="C1269" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/galpsn5lhwod1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="inlineStr">
+        <is>
+          <t>1fh4cpj</t>
+        </is>
+      </c>
+      <c r="B1270" t="inlineStr">
+        <is>
+          <t>If rust could ✨sparkle✨</t>
+        </is>
+      </c>
+      <c r="C1270" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a5fxbtjehwod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="inlineStr">
+        <is>
+          <t>1fh4455</t>
+        </is>
+      </c>
+      <c r="B1271" t="inlineStr">
+        <is>
+          <t>Holo Taco Waste of Space compared to ILNP Underground?</t>
+        </is>
+      </c>
+      <c r="C1271" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fh4455/holo_taco_waste_of_space_compared_to_ilnp/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="inlineStr">
+        <is>
+          <t>1fh3rbv</t>
+        </is>
+      </c>
+      <c r="B1272" t="inlineStr">
+        <is>
+          <t>Olive and June?</t>
+        </is>
+      </c>
+      <c r="C1272" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fh3rbv/olive_and_june/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" t="inlineStr">
+        <is>
+          <t>1fh35oo</t>
+        </is>
+      </c>
+      <c r="B1273" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Best and shiniest top coat? </t>
+        </is>
+      </c>
+      <c r="C1273" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fh35oo/best_and_shiniest_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" t="inlineStr">
+        <is>
+          <t>1fh338b</t>
+        </is>
+      </c>
+      <c r="B1274" t="inlineStr">
+        <is>
+          <t>Mayour InkPro collection: gel or regular polish?</t>
+        </is>
+      </c>
+      <c r="C1274" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fh338b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" t="inlineStr">
+        <is>
+          <t>1fh2fb8</t>
+        </is>
+      </c>
+      <c r="B1275" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Monarch Lacquer - Freeze Dance </t>
+        </is>
+      </c>
+      <c r="C1275" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fh2fb8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" t="inlineStr">
+        <is>
+          <t>1fh22pp</t>
+        </is>
+      </c>
+      <c r="B1276" t="inlineStr">
+        <is>
+          <t>First jelly sandwich!</t>
+        </is>
+      </c>
+      <c r="C1276" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a05w6miptvod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" t="inlineStr">
+        <is>
+          <t>1fh1xrh</t>
+        </is>
+      </c>
+      <c r="B1277" t="inlineStr">
+        <is>
+          <t>Anyone else's dog obsessed with nail polish?</t>
+        </is>
+      </c>
+      <c r="C1277" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fh1xrh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" t="inlineStr">
+        <is>
+          <t>1fh1k6z</t>
+        </is>
+      </c>
+      <c r="B1278" t="inlineStr">
+        <is>
+          <t>Phoenix Magical 🐦‍🔥✨</t>
+        </is>
+      </c>
+      <c r="C1278" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fh1k6z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" t="inlineStr">
+        <is>
+          <t>1fh1d0i</t>
+        </is>
+      </c>
+      <c r="B1279" t="inlineStr">
+        <is>
+          <t>Help identifying this indie</t>
+        </is>
+      </c>
+      <c r="C1279" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fh1d0i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" t="inlineStr">
+        <is>
+          <t>1fh0yhp</t>
+        </is>
+      </c>
+      <c r="B1280" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What do you do with nail polish you don't want? </t>
+        </is>
+      </c>
+      <c r="C1280" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fh0yhp/what_do_you_do_with_nail_polish_you_dont_want/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" t="inlineStr">
+        <is>
+          <t>1fh0ugr</t>
+        </is>
+      </c>
+      <c r="B1281" t="inlineStr">
+        <is>
+          <t>A pretty autumn holo-ish glitter by opi I can’t find the name of</t>
+        </is>
+      </c>
+      <c r="C1281" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fh0ugr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" t="inlineStr">
+        <is>
+          <t>1fh0mtn</t>
+        </is>
+      </c>
+      <c r="B1282" t="inlineStr">
+        <is>
+          <t>Dupe: Mooncat "Into the Wishing Well"</t>
+        </is>
+      </c>
+      <c r="C1282" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fh0mtn/dupe_mooncat_into_the_wishing_well/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" t="inlineStr">
+        <is>
+          <t>1fgztmc</t>
+        </is>
+      </c>
+      <c r="B1283" t="inlineStr">
+        <is>
+          <t>Shrek core</t>
+        </is>
+      </c>
+      <c r="C1283" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5d49vm9u7vod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" t="inlineStr">
+        <is>
+          <t>1fgzljl</t>
+        </is>
+      </c>
+      <c r="B1284" t="inlineStr">
+        <is>
+          <t>Has anyone tried travel watercolor brushes for cuticle oil?</t>
+        </is>
+      </c>
+      <c r="C1284" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fgzljl/has_anyone_tried_travel_watercolor_brushes_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" t="inlineStr">
+        <is>
+          <t>1fgzkkt</t>
+        </is>
+      </c>
+      <c r="B1285" t="inlineStr">
+        <is>
+          <t>neptune’s sand by mooncat ✨</t>
+        </is>
+      </c>
+      <c r="C1285" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k86s4e7l5vod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" t="inlineStr">
+        <is>
+          <t>1fgzgwp</t>
+        </is>
+      </c>
+      <c r="B1286" t="inlineStr">
+        <is>
+          <t>Dug this one out on a whim. I’m starstruck</t>
+        </is>
+      </c>
+      <c r="C1286" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fgzgwp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" t="inlineStr">
+        <is>
+          <t>1fgz9yd</t>
+        </is>
+      </c>
+      <c r="B1287" t="inlineStr">
+        <is>
+          <t>Any fix for badly damaged nail beds?</t>
+        </is>
+      </c>
+      <c r="C1287" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e71cpoyt2vod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" t="inlineStr">
+        <is>
+          <t>1fgytmr</t>
+        </is>
+      </c>
+      <c r="B1288" t="inlineStr">
+        <is>
+          <t>Shimmery Baby Poo</t>
+        </is>
+      </c>
+      <c r="C1288" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fgytmr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" t="inlineStr">
+        <is>
+          <t>1fgyfex</t>
+        </is>
+      </c>
+      <c r="B1289" t="inlineStr">
+        <is>
+          <t>It’s about that time 🍁🍂</t>
+        </is>
+      </c>
+      <c r="C1289" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tt3qw15dvuod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" t="inlineStr">
+        <is>
+          <t>1fgydb3</t>
+        </is>
+      </c>
+      <c r="B1290" t="inlineStr">
+        <is>
+          <t>Psilocybin is so shifty!</t>
+        </is>
+      </c>
+      <c r="C1290" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fgydb3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" t="inlineStr">
+        <is>
+          <t>1fgy9ql</t>
+        </is>
+      </c>
+      <c r="B1291" t="inlineStr">
+        <is>
+          <t>Recently left my career as a pastry chef</t>
+        </is>
+      </c>
+      <c r="C1291" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5jamefk2uuod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" t="inlineStr">
+        <is>
+          <t>1fgy9bk</t>
+        </is>
+      </c>
+      <c r="B1292" t="inlineStr">
+        <is>
+          <t>Poseidon’s prize🌊✨</t>
+        </is>
+      </c>
+      <c r="C1292" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/f3rp2iqytuod1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" t="inlineStr">
+        <is>
+          <t>1fgy24y</t>
+        </is>
+      </c>
+      <c r="B1293" t="inlineStr">
+        <is>
+          <t>Demure Halloween Colors</t>
+        </is>
+      </c>
+      <c r="C1293" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fgy24y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" t="inlineStr">
+        <is>
+          <t>1fgxu5b</t>
+        </is>
+      </c>
+      <c r="B1294" t="inlineStr">
+        <is>
+          <t>Dupes? 😮‍💨</t>
+        </is>
+      </c>
+      <c r="C1294" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/icx56zhdquod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" t="inlineStr">
+        <is>
+          <t>1fgxoxx</t>
+        </is>
+      </c>
+      <c r="B1295" t="inlineStr">
+        <is>
+          <t>Help- chipping / pealing nails</t>
+        </is>
+      </c>
+      <c r="C1295" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p7etw2p5puod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" t="inlineStr">
+        <is>
+          <t>1fgxgje</t>
+        </is>
+      </c>
+      <c r="B1296" t="inlineStr">
+        <is>
+          <t>Purple Slushie by Holo Taco again. Decided to do a video this time.</t>
+        </is>
+      </c>
+      <c r="C1296" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vl7p02j5nuod1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" t="inlineStr">
+        <is>
+          <t>1fgxcos</t>
+        </is>
+      </c>
+      <c r="B1297" t="inlineStr">
+        <is>
+          <t>Loving this combo!</t>
+        </is>
+      </c>
+      <c r="C1297" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fgxcos</t>
+        </is>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" t="inlineStr">
+        <is>
+          <t>1fgx8ic</t>
+        </is>
+      </c>
+      <c r="B1298" t="inlineStr">
+        <is>
+          <t>I looove this rusty red color! It’s just so perfect for autumn (:</t>
+        </is>
+      </c>
+      <c r="C1298" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/berlz0ifluod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" t="inlineStr">
+        <is>
+          <t>1fgwujw</t>
+        </is>
+      </c>
+      <c r="B1299" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fields of Elysium </t>
+        </is>
+      </c>
+      <c r="C1299" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1r1gv9r7iuod1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" t="inlineStr">
+        <is>
+          <t>1fgvvs3</t>
+        </is>
+      </c>
+      <c r="B1300" t="inlineStr">
+        <is>
+          <t xml:space="preserve">For those who asked to see my Psilocybin </t>
+        </is>
+      </c>
+      <c r="C1300" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fgvvs3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" t="inlineStr">
+        <is>
+          <t>1fgvmaz</t>
+        </is>
+      </c>
+      <c r="B1301" t="inlineStr">
+        <is>
+          <t>Pale pink neons? Night Owl Persist vs Atomic?</t>
+        </is>
+      </c>
+      <c r="C1301" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fgvmaz/pale_pink_neons_night_owl_persist_vs_atomic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" t="inlineStr">
+        <is>
+          <t>1fgubhr</t>
+        </is>
+      </c>
+      <c r="B1302" t="inlineStr">
+        <is>
+          <t>I've been really into Dany Vianna lately</t>
+        </is>
+      </c>
+      <c r="C1302" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2a8crr5wwtod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" t="inlineStr">
+        <is>
+          <t>1fgtcxl</t>
+        </is>
+      </c>
+      <c r="B1303" t="inlineStr">
+        <is>
+          <t>First time getting nail extensions I’m in love with these !</t>
+        </is>
+      </c>
+      <c r="C1303" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dczd3th4ptod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" t="inlineStr">
+        <is>
+          <t>1fgt11b</t>
+        </is>
+      </c>
+      <c r="B1304" t="inlineStr">
+        <is>
+          <t>Help with removing Lights Lacquer polish</t>
+        </is>
+      </c>
+      <c r="C1304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fgt11b/help_with_removing_lights_lacquer_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" t="inlineStr">
+        <is>
+          <t>1fgsray</t>
+        </is>
+      </c>
+      <c r="B1305" t="inlineStr">
+        <is>
+          <t>Tahitian Pearl Vibes ⚫</t>
+        </is>
+      </c>
+      <c r="C1305" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/yxjg4909jtod1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" t="inlineStr">
+        <is>
+          <t>1fgsn90</t>
+        </is>
+      </c>
+      <c r="B1306" t="inlineStr">
+        <is>
+          <t>Brickwall nails</t>
+        </is>
+      </c>
+      <c r="C1306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fgsn90</t>
+        </is>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" t="inlineStr">
+        <is>
+          <t>1fgshy2</t>
+        </is>
+      </c>
+      <c r="B1307" t="inlineStr">
+        <is>
+          <t>Top Bunk, Middle Bunk, Trundle Bed</t>
+        </is>
+      </c>
+      <c r="C1307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fgshy2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" t="inlineStr">
+        <is>
+          <t>1fgs8hq</t>
+        </is>
+      </c>
+      <c r="B1308" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sassy Sauce Verdigris is so pretty! </t>
+        </is>
+      </c>
+      <c r="C1308" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/biqpbuy6ftod1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1309">
+      <c r="A1309" t="inlineStr">
+        <is>
+          <t>1fgs7uu</t>
+        </is>
+      </c>
+      <c r="B1309" t="inlineStr">
+        <is>
+          <t>I finally developed the patience to sit through three coats of drying and not smudge my nails, but I don't have the patience to not trim this. Goodbyes are hard💔</t>
+        </is>
+      </c>
+      <c r="C1309" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ysejn2k1ftod1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1310">
+      <c r="A1310" t="inlineStr">
+        <is>
+          <t>1fgrutr</t>
+        </is>
+      </c>
+      <c r="B1310" t="inlineStr">
+        <is>
+          <t xml:space="preserve">One peeling nail - short term fix? </t>
+        </is>
+      </c>
+      <c r="C1310" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t4rp3i76ctod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1311">
+      <c r="A1311" t="inlineStr">
+        <is>
+          <t>1fgrsra</t>
+        </is>
+      </c>
+      <c r="B1311" t="inlineStr">
+        <is>
+          <t>Salon Perfect Flash Reflective Glitter polish dries so quickly and gritty?</t>
+        </is>
+      </c>
+      <c r="C1311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fgrsra/salon_perfect_flash_reflective_glitter_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1312">
+      <c r="A1312" t="inlineStr">
+        <is>
+          <t>1fgrsgq</t>
+        </is>
+      </c>
+      <c r="B1312" t="inlineStr">
+        <is>
+          <t>🧪🌈✨Nail Polish Science: the Chemistry of Colour✨🌈🧪</t>
+        </is>
+      </c>
+      <c r="C1312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fgrsgq/nail_polish_science_the_chemistry_of_colour/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1313">
+      <c r="A1313" t="inlineStr">
+        <is>
+          <t>1fgrsed</t>
+        </is>
+      </c>
+      <c r="B1313" t="inlineStr">
+        <is>
+          <t>Can I just paint over my current manicure?</t>
+        </is>
+      </c>
+      <c r="C1313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fgrsed/can_i_just_paint_over_my_current_manicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1314">
+      <c r="A1314" t="inlineStr">
+        <is>
+          <t>1fgrpam</t>
+        </is>
+      </c>
+      <c r="B1314" t="inlineStr">
+        <is>
+          <t>Already chipped one but still loving this color!</t>
+        </is>
+      </c>
+      <c r="C1314" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fgrpam</t>
+        </is>
+      </c>
+    </row>
+    <row r="1315">
+      <c r="A1315" t="inlineStr">
+        <is>
+          <t>1fgrow0</t>
+        </is>
+      </c>
+      <c r="B1315" t="inlineStr">
+        <is>
+          <t>Mermaid Nails</t>
+        </is>
+      </c>
+      <c r="C1315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fgrow0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1316">
+      <c r="A1316" t="inlineStr">
+        <is>
+          <t>1fgrkun</t>
+        </is>
+      </c>
+      <c r="B1316" t="inlineStr">
+        <is>
+          <t>Sloppy Holo Taco velvet Menchie Cat Eye</t>
+        </is>
+      </c>
+      <c r="C1316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fgrkun</t>
+        </is>
+      </c>
+    </row>
+    <row r="1317">
+      <c r="A1317" t="inlineStr">
+        <is>
+          <t>1fgr9iu</t>
+        </is>
+      </c>
+      <c r="B1317" t="inlineStr">
+        <is>
+          <t>Matching my drawing (and some other manis)</t>
+        </is>
+      </c>
+      <c r="C1317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fgr9iu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1318">
+      <c r="A1318" t="inlineStr">
+        <is>
+          <t>1fgr0px</t>
+        </is>
+      </c>
+      <c r="B1318" t="inlineStr">
+        <is>
+          <t>Psilocybin 🍄</t>
+        </is>
+      </c>
+      <c r="C1318" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fgr0px</t>
+        </is>
+      </c>
+    </row>
+    <row r="1319">
+      <c r="A1319" t="inlineStr">
+        <is>
+          <t>1fgptia</t>
+        </is>
+      </c>
+      <c r="B1319" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Anyone else disappointed that all the bottles can’t look the exact same? </t>
+        </is>
+      </c>
+      <c r="C1319" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2p4jfexrvsod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1320">
+      <c r="A1320" t="inlineStr">
+        <is>
+          <t>1fgpn8u</t>
+        </is>
+      </c>
+      <c r="B1320" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Thermal from 2016 still working! </t>
+        </is>
+      </c>
+      <c r="C1320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fgpn8u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1321">
+      <c r="A1321" t="inlineStr">
+        <is>
+          <t>1fgoxf3</t>
+        </is>
+      </c>
+      <c r="B1321" t="inlineStr">
+        <is>
+          <t>First Mooncat polish ✨ Illusionist</t>
+        </is>
+      </c>
+      <c r="C1321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fgoxf3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1322">
+      <c r="A1322" t="inlineStr">
+        <is>
+          <t>1fgoo0l</t>
+        </is>
+      </c>
+      <c r="B1322" t="inlineStr">
+        <is>
+          <t>But Do Aliens Believe In Me?</t>
+        </is>
+      </c>
+      <c r="C1322" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/v6swfjtomsod1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1323">
+      <c r="A1323" t="inlineStr">
+        <is>
+          <t>1fgnlru</t>
+        </is>
+      </c>
+      <c r="B1323" t="inlineStr">
+        <is>
+          <t>Break held together by polish</t>
+        </is>
+      </c>
+      <c r="C1323" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w9pxbyg7esod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1324">
+      <c r="A1324" t="inlineStr">
+        <is>
+          <t>1fgnlqi</t>
+        </is>
+      </c>
+      <c r="B1324" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Girl Dragon </t>
+        </is>
+      </c>
+      <c r="C1324" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fgnlqi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1325">
+      <c r="A1325" t="inlineStr">
+        <is>
+          <t>1fgmxoy</t>
+        </is>
+      </c>
+      <c r="B1325" t="inlineStr">
+        <is>
+          <t>I bought these in the same purchase 🫡</t>
+        </is>
+      </c>
+      <c r="C1325" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/46mbta2o8sod1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1326">
+      <c r="A1326" t="inlineStr">
+        <is>
+          <t>1fgmodw</t>
+        </is>
+      </c>
+      <c r="B1326" t="inlineStr">
+        <is>
+          <t>Nails perfectly match</t>
+        </is>
+      </c>
+      <c r="C1326" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fgmodw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1327">
+      <c r="A1327" t="inlineStr">
+        <is>
+          <t>1fglu7p</t>
+        </is>
+      </c>
+      <c r="B1327" t="inlineStr">
+        <is>
+          <t>Glam Polish “I Wanna Dance With Somebody” is an actual party on my nails ✨</t>
+        </is>
+      </c>
+      <c r="C1327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fgltum</t>
+        </is>
+      </c>
+    </row>
+    <row r="1328">
+      <c r="A1328" t="inlineStr">
+        <is>
+          <t>1fgldkb</t>
+        </is>
+      </c>
+      <c r="B1328" t="inlineStr">
+        <is>
+          <t>Sabertooth 🩵🩵</t>
+        </is>
+      </c>
+      <c r="C1328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fgldkb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1329">
+      <c r="A1329" t="inlineStr">
+        <is>
+          <t>1fgklrk</t>
+        </is>
+      </c>
+      <c r="B1329" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Just picked up Rogue Lacquer’s So Franken Cute in hopes that it’s a sufficient dupe of the Sour Apple Rings I never got my hands on </t>
+        </is>
+      </c>
+      <c r="C1329" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fgklrk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1330">
+      <c r="A1330" t="inlineStr">
+        <is>
+          <t>1fgjj9r</t>
+        </is>
+      </c>
+      <c r="B1330" t="inlineStr">
+        <is>
+          <t>jello jello peel off set in europe (or alternative?)</t>
+        </is>
+      </c>
+      <c r="C1330" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fgjj9r/jello_jello_peel_off_set_in_europe_or_alternative/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1331">
+      <c r="A1331" t="inlineStr">
+        <is>
+          <t>1fghcpy</t>
+        </is>
+      </c>
+      <c r="B1331" t="inlineStr">
+        <is>
+          <t>Lights Lacquer haul!!</t>
+        </is>
+      </c>
+      <c r="C1331" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ujierbyghqod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1332">
+      <c r="A1332" t="inlineStr">
+        <is>
+          <t>1fh7k7v</t>
+        </is>
+      </c>
+      <c r="B1332" t="inlineStr">
+        <is>
+          <t>Barbie pink and a star</t>
+        </is>
+      </c>
+      <c r="C1332" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qymlv5sxkxod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1333">
+      <c r="A1333" t="inlineStr">
+        <is>
+          <t>1fh20co</t>
+        </is>
+      </c>
+      <c r="B1333" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Matte cat eye + chrome eyes </t>
+        </is>
+      </c>
+      <c r="C1333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fh20co</t>
+        </is>
+      </c>
+    </row>
+    <row r="1334">
+      <c r="A1334" t="inlineStr">
+        <is>
+          <t>1fgw5t4</t>
+        </is>
+      </c>
+      <c r="B1334" t="inlineStr">
+        <is>
+          <t>I’m obsessed with how my sister’s nails came out 🫶🏽</t>
+        </is>
+      </c>
+      <c r="C1334" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p79ixnnmcuod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1335">
+      <c r="A1335" t="inlineStr">
+        <is>
+          <t>1fgvl92</t>
+        </is>
+      </c>
+      <c r="B1335" t="inlineStr">
+        <is>
+          <t>I heard you like magic🪄🎩🐇✨</t>
+        </is>
+      </c>
+      <c r="C1335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fgvl92</t>
+        </is>
+      </c>
+    </row>
+    <row r="1336">
+      <c r="A1336" t="inlineStr">
+        <is>
+          <t>1fgv71w</t>
+        </is>
+      </c>
+      <c r="B1336" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time nail art </t>
+        </is>
+      </c>
+      <c r="C1336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fgv71w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1337">
+      <c r="A1337" t="inlineStr">
+        <is>
+          <t>1fgubi2</t>
+        </is>
+      </c>
+      <c r="B1337" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What do you think of my nails? </t>
+        </is>
+      </c>
+      <c r="C1337" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2gzy5ecywtod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1338">
+      <c r="A1338" t="inlineStr">
+        <is>
+          <t>1fgtac7</t>
+        </is>
+      </c>
+      <c r="B1338" t="inlineStr">
+        <is>
+          <t>Mermaid seashell nails 🧜‍♀️🐚✨</t>
+        </is>
+      </c>
+      <c r="C1338" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8lmnn2kmotod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1339">
+      <c r="A1339" t="inlineStr">
+        <is>
+          <t>1fgstg0</t>
+        </is>
+      </c>
+      <c r="B1339" t="inlineStr">
+        <is>
+          <t>How do I get the gold flakes out and keep the design underneath?</t>
+        </is>
+      </c>
+      <c r="C1339" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fgstg0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1340">
+      <c r="A1340" t="inlineStr">
+        <is>
+          <t>1fgsi63</t>
+        </is>
+      </c>
+      <c r="B1340" t="inlineStr">
+        <is>
+          <t xml:space="preserve">about to remove my grown out nails but decided to share first </t>
+        </is>
+      </c>
+      <c r="C1340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fgsi63</t>
+        </is>
+      </c>
+    </row>
+    <row r="1341">
+      <c r="A1341" t="inlineStr">
+        <is>
+          <t>1fgr23g</t>
+        </is>
+      </c>
+      <c r="B1341" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time trying nail art and frustrated! </t>
+        </is>
+      </c>
+      <c r="C1341" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d37e6h1t5tod1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1342">
+      <c r="A1342" t="inlineStr">
+        <is>
+          <t>1fgk38u</t>
+        </is>
+      </c>
+      <c r="B1342" t="inlineStr">
+        <is>
+          <t xml:space="preserve">along came a spider and made my nail pretty♥ </t>
+        </is>
+      </c>
+      <c r="C1342" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/75g55g7mhrod1.png</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>